<commit_message>
feat: update Sekolah and User models; refactor relationships and migration structure; remove UserProfile model
</commit_message>
<xml_diff>
--- a/public/siswas/Data_Siswa.xlsx
+++ b/public/siswas/Data_Siswa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\DELL\Local C Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Herd\mvp\public\siswas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594DA326-42DF-4D5A-80EA-F617015E24E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CA13FE-F6DD-492B-88DF-23A8940E5918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EC150BA0-A7DA-9543-9030-8FC30C50B5C6}"/>
   </bookViews>
@@ -6098,10 +6098,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2656"/>
+  <dimension ref="A1:D1890"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A1878" workbookViewId="0">
+      <selection activeCell="A1891" sqref="A1891:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -32572,2796 +32572,8 @@
         <v>20542392</v>
       </c>
     </row>
-    <row r="1891" spans="1:4" ht="12.75">
-      <c r="C1891" s="2"/>
-    </row>
-    <row r="1892" spans="1:4" ht="12.75">
-      <c r="C1892" s="2"/>
-    </row>
-    <row r="1893" spans="1:4" ht="12.75">
-      <c r="C1893" s="2"/>
-    </row>
-    <row r="1894" spans="1:4" ht="12.75">
-      <c r="C1894" s="2"/>
-    </row>
-    <row r="1895" spans="1:4" ht="12.75">
-      <c r="C1895" s="2"/>
-    </row>
-    <row r="1896" spans="1:4" ht="12.75">
-      <c r="C1896" s="2"/>
-    </row>
-    <row r="1897" spans="1:4" ht="12.75">
-      <c r="C1897" s="2"/>
-    </row>
-    <row r="1898" spans="1:4" ht="12.75">
-      <c r="C1898" s="2"/>
-    </row>
-    <row r="1899" spans="1:4" ht="12.75">
-      <c r="C1899" s="2"/>
-    </row>
-    <row r="1900" spans="1:4" ht="12.75">
-      <c r="C1900" s="2"/>
-    </row>
-    <row r="1901" spans="1:4" ht="12.75">
-      <c r="C1901" s="2"/>
-    </row>
-    <row r="1902" spans="1:4" ht="12.75">
-      <c r="C1902" s="2"/>
-    </row>
-    <row r="1903" spans="1:4" ht="12.75">
-      <c r="C1903" s="2"/>
-    </row>
-    <row r="1904" spans="1:4" ht="12.75">
-      <c r="C1904" s="2"/>
-    </row>
-    <row r="1905" spans="3:3" ht="12.75">
-      <c r="C1905" s="2"/>
-    </row>
-    <row r="1906" spans="3:3" ht="12.75">
-      <c r="C1906" s="2"/>
-    </row>
-    <row r="1907" spans="3:3" ht="12.75">
-      <c r="C1907" s="2"/>
-    </row>
-    <row r="1908" spans="3:3" ht="12.75">
-      <c r="C1908" s="2"/>
-    </row>
-    <row r="1909" spans="3:3" ht="12.75">
-      <c r="C1909" s="2"/>
-    </row>
-    <row r="1910" spans="3:3" ht="12.75">
-      <c r="C1910" s="2"/>
-    </row>
-    <row r="1911" spans="3:3" ht="12.75">
-      <c r="C1911" s="2"/>
-    </row>
-    <row r="1912" spans="3:3" ht="12.75">
-      <c r="C1912" s="2"/>
-    </row>
-    <row r="1913" spans="3:3" ht="12.75">
-      <c r="C1913" s="2"/>
-    </row>
-    <row r="1914" spans="3:3" ht="12.75">
-      <c r="C1914" s="2"/>
-    </row>
-    <row r="1915" spans="3:3" ht="12.75">
-      <c r="C1915" s="2"/>
-    </row>
-    <row r="1916" spans="3:3" ht="12.75">
-      <c r="C1916" s="2"/>
-    </row>
-    <row r="1917" spans="3:3" ht="12.75">
-      <c r="C1917" s="2"/>
-    </row>
-    <row r="1918" spans="3:3" ht="12.75">
-      <c r="C1918" s="2"/>
-    </row>
-    <row r="1919" spans="3:3" ht="12.75">
-      <c r="C1919" s="2"/>
-    </row>
-    <row r="1920" spans="3:3" ht="12.75">
-      <c r="C1920" s="2"/>
-    </row>
-    <row r="1921" spans="3:3" ht="12.75">
-      <c r="C1921" s="2"/>
-    </row>
-    <row r="1922" spans="3:3" ht="12.75">
-      <c r="C1922" s="2"/>
-    </row>
-    <row r="1923" spans="3:3" ht="12.75">
-      <c r="C1923" s="2"/>
-    </row>
-    <row r="1924" spans="3:3" ht="12.75">
-      <c r="C1924" s="2"/>
-    </row>
-    <row r="1925" spans="3:3" ht="12.75">
-      <c r="C1925" s="2"/>
-    </row>
-    <row r="1926" spans="3:3" ht="12.75">
-      <c r="C1926" s="2"/>
-    </row>
-    <row r="1927" spans="3:3" ht="12.75">
-      <c r="C1927" s="2"/>
-    </row>
-    <row r="1928" spans="3:3" ht="12.75">
-      <c r="C1928" s="2"/>
-    </row>
-    <row r="1929" spans="3:3" ht="12.75">
-      <c r="C1929" s="2"/>
-    </row>
-    <row r="1930" spans="3:3" ht="12.75">
-      <c r="C1930" s="2"/>
-    </row>
-    <row r="1931" spans="3:3" ht="12.75">
-      <c r="C1931" s="2"/>
-    </row>
-    <row r="1932" spans="3:3" ht="12.75">
-      <c r="C1932" s="2"/>
-    </row>
-    <row r="1933" spans="3:3" ht="12.75">
-      <c r="C1933" s="2"/>
-    </row>
-    <row r="1934" spans="3:3" ht="12.75">
-      <c r="C1934" s="2"/>
-    </row>
-    <row r="1935" spans="3:3" ht="12.75">
-      <c r="C1935" s="2"/>
-    </row>
-    <row r="1936" spans="3:3" ht="12.75">
-      <c r="C1936" s="2"/>
-    </row>
-    <row r="1937" spans="3:3" ht="12.75">
-      <c r="C1937" s="2"/>
-    </row>
-    <row r="1938" spans="3:3" ht="12.75">
-      <c r="C1938" s="2"/>
-    </row>
-    <row r="1939" spans="3:3" ht="12.75">
-      <c r="C1939" s="2"/>
-    </row>
-    <row r="1940" spans="3:3" ht="12.75">
-      <c r="C1940" s="2"/>
-    </row>
-    <row r="1941" spans="3:3" ht="12.75">
-      <c r="C1941" s="2"/>
-    </row>
-    <row r="1942" spans="3:3" ht="12.75">
-      <c r="C1942" s="2"/>
-    </row>
-    <row r="1943" spans="3:3" ht="12.75">
-      <c r="C1943" s="2"/>
-    </row>
-    <row r="1944" spans="3:3" ht="12.75">
-      <c r="C1944" s="2"/>
-    </row>
-    <row r="1945" spans="3:3" ht="12.75">
-      <c r="C1945" s="2"/>
-    </row>
-    <row r="1946" spans="3:3" ht="12.75">
-      <c r="C1946" s="2"/>
-    </row>
-    <row r="1947" spans="3:3" ht="12.75">
-      <c r="C1947" s="2"/>
-    </row>
-    <row r="1948" spans="3:3" ht="12.75">
-      <c r="C1948" s="2"/>
-    </row>
-    <row r="1949" spans="3:3" ht="12.75">
-      <c r="C1949" s="2"/>
-    </row>
-    <row r="1950" spans="3:3" ht="12.75">
-      <c r="C1950" s="2"/>
-    </row>
-    <row r="1951" spans="3:3" ht="12.75">
-      <c r="C1951" s="2"/>
-    </row>
-    <row r="1952" spans="3:3" ht="12.75">
-      <c r="C1952" s="2"/>
-    </row>
-    <row r="1953" spans="3:3" ht="12.75">
-      <c r="C1953" s="2"/>
-    </row>
-    <row r="1954" spans="3:3" ht="12.75">
-      <c r="C1954" s="2"/>
-    </row>
-    <row r="1955" spans="3:3" ht="12.75">
-      <c r="C1955" s="2"/>
-    </row>
-    <row r="1956" spans="3:3" ht="12.75">
-      <c r="C1956" s="2"/>
-    </row>
-    <row r="1957" spans="3:3" ht="12.75">
-      <c r="C1957" s="2"/>
-    </row>
-    <row r="1958" spans="3:3" ht="12.75">
-      <c r="C1958" s="2"/>
-    </row>
-    <row r="1959" spans="3:3" ht="12.75">
-      <c r="C1959" s="2"/>
-    </row>
-    <row r="1960" spans="3:3" ht="12.75">
-      <c r="C1960" s="2"/>
-    </row>
-    <row r="1961" spans="3:3" ht="12.75">
-      <c r="C1961" s="2"/>
-    </row>
-    <row r="1962" spans="3:3" ht="12.75">
-      <c r="C1962" s="2"/>
-    </row>
-    <row r="1963" spans="3:3" ht="12.75">
-      <c r="C1963" s="2"/>
-    </row>
-    <row r="1964" spans="3:3" ht="12.75">
-      <c r="C1964" s="2"/>
-    </row>
-    <row r="1965" spans="3:3" ht="12.75">
-      <c r="C1965" s="2"/>
-    </row>
-    <row r="1966" spans="3:3" ht="12.75">
-      <c r="C1966" s="2"/>
-    </row>
-    <row r="1967" spans="3:3" ht="12.75">
-      <c r="C1967" s="2"/>
-    </row>
-    <row r="1968" spans="3:3" ht="12.75">
-      <c r="C1968" s="2"/>
-    </row>
-    <row r="1969" spans="3:3" ht="12.75">
-      <c r="C1969" s="2"/>
-    </row>
-    <row r="1970" spans="3:3" ht="12.75">
-      <c r="C1970" s="2"/>
-    </row>
-    <row r="1971" spans="3:3" ht="12.75">
-      <c r="C1971" s="2"/>
-    </row>
-    <row r="1972" spans="3:3" ht="12.75">
-      <c r="C1972" s="2"/>
-    </row>
-    <row r="1973" spans="3:3" ht="12.75">
-      <c r="C1973" s="2"/>
-    </row>
-    <row r="1974" spans="3:3" ht="12.75">
-      <c r="C1974" s="2"/>
-    </row>
-    <row r="1975" spans="3:3" ht="12.75">
-      <c r="C1975" s="2"/>
-    </row>
-    <row r="1976" spans="3:3" ht="12.75">
-      <c r="C1976" s="2"/>
-    </row>
-    <row r="1977" spans="3:3" ht="12.75">
-      <c r="C1977" s="2"/>
-    </row>
-    <row r="1978" spans="3:3" ht="12.75">
-      <c r="C1978" s="2"/>
-    </row>
-    <row r="1979" spans="3:3" ht="12.75">
-      <c r="C1979" s="2"/>
-    </row>
-    <row r="1980" spans="3:3" ht="12.75">
-      <c r="C1980" s="2"/>
-    </row>
-    <row r="1981" spans="3:3" ht="12.75">
-      <c r="C1981" s="2"/>
-    </row>
-    <row r="1982" spans="3:3" ht="12.75">
-      <c r="C1982" s="2"/>
-    </row>
-    <row r="1983" spans="3:3" ht="12.75">
-      <c r="C1983" s="2"/>
-    </row>
-    <row r="1984" spans="3:3" ht="12.75">
-      <c r="C1984" s="2"/>
-    </row>
-    <row r="1985" spans="3:3" ht="12.75">
-      <c r="C1985" s="2"/>
-    </row>
-    <row r="1986" spans="3:3" ht="12.75">
-      <c r="C1986" s="2"/>
-    </row>
-    <row r="1987" spans="3:3" ht="12.75">
-      <c r="C1987" s="2"/>
-    </row>
-    <row r="1988" spans="3:3" ht="12.75">
-      <c r="C1988" s="2"/>
-    </row>
-    <row r="1989" spans="3:3" ht="12.75">
-      <c r="C1989" s="2"/>
-    </row>
-    <row r="1990" spans="3:3" ht="12.75">
-      <c r="C1990" s="2"/>
-    </row>
-    <row r="1991" spans="3:3" ht="12.75">
-      <c r="C1991" s="2"/>
-    </row>
-    <row r="1992" spans="3:3" ht="12.75">
-      <c r="C1992" s="2"/>
-    </row>
-    <row r="1993" spans="3:3" ht="12.75">
-      <c r="C1993" s="2"/>
-    </row>
-    <row r="1994" spans="3:3" ht="12.75">
-      <c r="C1994" s="2"/>
-    </row>
-    <row r="1995" spans="3:3" ht="12.75">
-      <c r="C1995" s="2"/>
-    </row>
-    <row r="1996" spans="3:3" ht="12.75">
-      <c r="C1996" s="2"/>
-    </row>
-    <row r="1997" spans="3:3" ht="12.75">
-      <c r="C1997" s="2"/>
-    </row>
-    <row r="1998" spans="3:3" ht="12.75">
-      <c r="C1998" s="2"/>
-    </row>
-    <row r="1999" spans="3:3" ht="12.75">
-      <c r="C1999" s="2"/>
-    </row>
-    <row r="2000" spans="3:3" ht="12.75">
-      <c r="C2000" s="2"/>
-    </row>
-    <row r="2001" spans="3:3" ht="12.75">
-      <c r="C2001" s="2"/>
-    </row>
-    <row r="2002" spans="3:3" ht="12.75">
-      <c r="C2002" s="2"/>
-    </row>
-    <row r="2003" spans="3:3" ht="12.75">
-      <c r="C2003" s="2"/>
-    </row>
-    <row r="2004" spans="3:3" ht="12.75">
-      <c r="C2004" s="2"/>
-    </row>
-    <row r="2005" spans="3:3" ht="12.75">
-      <c r="C2005" s="2"/>
-    </row>
-    <row r="2006" spans="3:3" ht="12.75">
-      <c r="C2006" s="2"/>
-    </row>
-    <row r="2007" spans="3:3" ht="12.75">
-      <c r="C2007" s="2"/>
-    </row>
-    <row r="2008" spans="3:3" ht="12.75">
-      <c r="C2008" s="2"/>
-    </row>
-    <row r="2009" spans="3:3" ht="12.75">
-      <c r="C2009" s="2"/>
-    </row>
-    <row r="2010" spans="3:3" ht="12.75">
-      <c r="C2010" s="2"/>
-    </row>
-    <row r="2011" spans="3:3" ht="12.75">
-      <c r="C2011" s="2"/>
-    </row>
-    <row r="2012" spans="3:3" ht="12.75">
-      <c r="C2012" s="2"/>
-    </row>
-    <row r="2013" spans="3:3" ht="12.75">
-      <c r="C2013" s="2"/>
-    </row>
-    <row r="2014" spans="3:3" ht="12.75">
-      <c r="C2014" s="2"/>
-    </row>
-    <row r="2015" spans="3:3" ht="12.75">
-      <c r="C2015" s="2"/>
-    </row>
-    <row r="2016" spans="3:3" ht="12.75">
-      <c r="C2016" s="2"/>
-    </row>
-    <row r="2017" spans="3:3" ht="12.75">
-      <c r="C2017" s="2"/>
-    </row>
-    <row r="2018" spans="3:3" ht="12.75">
-      <c r="C2018" s="2"/>
-    </row>
-    <row r="2019" spans="3:3" ht="12.75">
-      <c r="C2019" s="2"/>
-    </row>
-    <row r="2020" spans="3:3" ht="12.75">
-      <c r="C2020" s="2"/>
-    </row>
-    <row r="2021" spans="3:3" ht="12.75">
-      <c r="C2021" s="2"/>
-    </row>
-    <row r="2022" spans="3:3" ht="12.75">
-      <c r="C2022" s="2"/>
-    </row>
-    <row r="2023" spans="3:3" ht="12.75">
-      <c r="C2023" s="2"/>
-    </row>
-    <row r="2024" spans="3:3" ht="12.75">
-      <c r="C2024" s="2"/>
-    </row>
-    <row r="2025" spans="3:3" ht="12.75">
-      <c r="C2025" s="2"/>
-    </row>
-    <row r="2026" spans="3:3" ht="12.75">
-      <c r="C2026" s="2"/>
-    </row>
-    <row r="2027" spans="3:3" ht="12.75">
-      <c r="C2027" s="2"/>
-    </row>
-    <row r="2028" spans="3:3" ht="12.75">
-      <c r="C2028" s="2"/>
-    </row>
-    <row r="2029" spans="3:3" ht="12.75">
-      <c r="C2029" s="2"/>
-    </row>
-    <row r="2030" spans="3:3" ht="12.75">
-      <c r="C2030" s="2"/>
-    </row>
-    <row r="2031" spans="3:3" ht="12.75">
-      <c r="C2031" s="2"/>
-    </row>
-    <row r="2032" spans="3:3" ht="12.75">
-      <c r="C2032" s="2"/>
-    </row>
-    <row r="2033" spans="3:3" ht="12.75">
-      <c r="C2033" s="2"/>
-    </row>
-    <row r="2034" spans="3:3" ht="12.75">
-      <c r="C2034" s="2"/>
-    </row>
-    <row r="2035" spans="3:3" ht="12.75">
-      <c r="C2035" s="2"/>
-    </row>
-    <row r="2036" spans="3:3" ht="12.75">
-      <c r="C2036" s="2"/>
-    </row>
-    <row r="2037" spans="3:3" ht="12.75">
-      <c r="C2037" s="2"/>
-    </row>
-    <row r="2038" spans="3:3" ht="12.75">
-      <c r="C2038" s="2"/>
-    </row>
-    <row r="2039" spans="3:3" ht="12.75">
-      <c r="C2039" s="2"/>
-    </row>
-    <row r="2040" spans="3:3" ht="12.75">
-      <c r="C2040" s="2"/>
-    </row>
-    <row r="2041" spans="3:3" ht="12.75">
-      <c r="C2041" s="2"/>
-    </row>
-    <row r="2042" spans="3:3" ht="12.75">
-      <c r="C2042" s="2"/>
-    </row>
-    <row r="2043" spans="3:3" ht="12.75">
-      <c r="C2043" s="2"/>
-    </row>
-    <row r="2044" spans="3:3" ht="12.75">
-      <c r="C2044" s="2"/>
-    </row>
-    <row r="2045" spans="3:3" ht="12.75">
-      <c r="C2045" s="2"/>
-    </row>
-    <row r="2046" spans="3:3" ht="12.75">
-      <c r="C2046" s="2"/>
-    </row>
-    <row r="2047" spans="3:3" ht="12.75">
-      <c r="C2047" s="2"/>
-    </row>
-    <row r="2048" spans="3:3" ht="12.75">
-      <c r="C2048" s="2"/>
-    </row>
-    <row r="2049" spans="3:3" ht="12.75">
-      <c r="C2049" s="2"/>
-    </row>
-    <row r="2050" spans="3:3" ht="12.75">
-      <c r="C2050" s="2"/>
-    </row>
-    <row r="2051" spans="3:3" ht="12.75">
-      <c r="C2051" s="2"/>
-    </row>
-    <row r="2052" spans="3:3" ht="12.75">
-      <c r="C2052" s="2"/>
-    </row>
-    <row r="2053" spans="3:3" ht="12.75">
-      <c r="C2053" s="2"/>
-    </row>
-    <row r="2054" spans="3:3" ht="12.75">
-      <c r="C2054" s="2"/>
-    </row>
-    <row r="2055" spans="3:3" ht="12.75">
-      <c r="C2055" s="2"/>
-    </row>
-    <row r="2056" spans="3:3" ht="12.75">
-      <c r="C2056" s="2"/>
-    </row>
-    <row r="2057" spans="3:3" ht="12.75">
-      <c r="C2057" s="2"/>
-    </row>
-    <row r="2058" spans="3:3" ht="12.75">
-      <c r="C2058" s="2"/>
-    </row>
-    <row r="2059" spans="3:3" ht="12.75">
-      <c r="C2059" s="2"/>
-    </row>
-    <row r="2060" spans="3:3" ht="12.75">
-      <c r="C2060" s="2"/>
-    </row>
-    <row r="2061" spans="3:3" ht="12.75">
-      <c r="C2061" s="2"/>
-    </row>
-    <row r="2062" spans="3:3" ht="12.75">
-      <c r="C2062" s="2"/>
-    </row>
-    <row r="2063" spans="3:3" ht="12.75">
-      <c r="C2063" s="2"/>
-    </row>
-    <row r="2064" spans="3:3" ht="12.75">
-      <c r="C2064" s="2"/>
-    </row>
-    <row r="2065" spans="3:3" ht="12.75">
-      <c r="C2065" s="2"/>
-    </row>
-    <row r="2066" spans="3:3" ht="12.75">
-      <c r="C2066" s="2"/>
-    </row>
-    <row r="2067" spans="3:3" ht="12.75">
-      <c r="C2067" s="2"/>
-    </row>
-    <row r="2068" spans="3:3" ht="12.75">
-      <c r="C2068" s="2"/>
-    </row>
-    <row r="2069" spans="3:3" ht="12.75">
-      <c r="C2069" s="2"/>
-    </row>
-    <row r="2070" spans="3:3" ht="12.75">
-      <c r="C2070" s="2"/>
-    </row>
-    <row r="2071" spans="3:3" ht="12.75">
-      <c r="C2071" s="2"/>
-    </row>
-    <row r="2072" spans="3:3" ht="12.75">
-      <c r="C2072" s="2"/>
-    </row>
-    <row r="2073" spans="3:3" ht="12.75">
-      <c r="C2073" s="2"/>
-    </row>
-    <row r="2074" spans="3:3" ht="12.75">
-      <c r="C2074" s="2"/>
-    </row>
-    <row r="2075" spans="3:3" ht="12.75">
-      <c r="C2075" s="2"/>
-    </row>
-    <row r="2076" spans="3:3" ht="12.75">
-      <c r="C2076" s="2"/>
-    </row>
-    <row r="2077" spans="3:3" ht="12.75">
-      <c r="C2077" s="2"/>
-    </row>
-    <row r="2078" spans="3:3" ht="12.75">
-      <c r="C2078" s="2"/>
-    </row>
-    <row r="2079" spans="3:3" ht="12.75">
-      <c r="C2079" s="2"/>
-    </row>
-    <row r="2080" spans="3:3" ht="12.75">
-      <c r="C2080" s="2"/>
-    </row>
-    <row r="2081" spans="3:3" ht="12.75">
-      <c r="C2081" s="2"/>
-    </row>
-    <row r="2082" spans="3:3" ht="12.75">
-      <c r="C2082" s="2"/>
-    </row>
-    <row r="2083" spans="3:3" ht="12.75">
-      <c r="C2083" s="2"/>
-    </row>
-    <row r="2084" spans="3:3" ht="12.75">
-      <c r="C2084" s="2"/>
-    </row>
-    <row r="2085" spans="3:3" ht="12.75">
-      <c r="C2085" s="2"/>
-    </row>
-    <row r="2086" spans="3:3" ht="12.75">
-      <c r="C2086" s="2"/>
-    </row>
-    <row r="2087" spans="3:3" ht="12.75">
-      <c r="C2087" s="2"/>
-    </row>
-    <row r="2088" spans="3:3" ht="12.75">
-      <c r="C2088" s="2"/>
-    </row>
-    <row r="2089" spans="3:3" ht="12.75">
-      <c r="C2089" s="2"/>
-    </row>
-    <row r="2090" spans="3:3" ht="12.75">
-      <c r="C2090" s="2"/>
-    </row>
-    <row r="2091" spans="3:3" ht="12.75">
-      <c r="C2091" s="2"/>
-    </row>
-    <row r="2092" spans="3:3" ht="12.75">
-      <c r="C2092" s="2"/>
-    </row>
-    <row r="2093" spans="3:3" ht="12.75">
-      <c r="C2093" s="2"/>
-    </row>
-    <row r="2094" spans="3:3" ht="12.75">
-      <c r="C2094" s="2"/>
-    </row>
-    <row r="2095" spans="3:3" ht="12.75">
-      <c r="C2095" s="2"/>
-    </row>
-    <row r="2096" spans="3:3" ht="12.75">
-      <c r="C2096" s="2"/>
-    </row>
-    <row r="2097" spans="3:3" ht="12.75">
-      <c r="C2097" s="2"/>
-    </row>
-    <row r="2098" spans="3:3" ht="12.75">
-      <c r="C2098" s="2"/>
-    </row>
-    <row r="2099" spans="3:3" ht="12.75">
-      <c r="C2099" s="2"/>
-    </row>
-    <row r="2100" spans="3:3" ht="12.75">
-      <c r="C2100" s="2"/>
-    </row>
-    <row r="2101" spans="3:3" ht="12.75">
-      <c r="C2101" s="2"/>
-    </row>
-    <row r="2102" spans="3:3" ht="12.75">
-      <c r="C2102" s="2"/>
-    </row>
-    <row r="2103" spans="3:3" ht="12.75">
-      <c r="C2103" s="2"/>
-    </row>
-    <row r="2104" spans="3:3" ht="12.75">
-      <c r="C2104" s="2"/>
-    </row>
-    <row r="2105" spans="3:3" ht="12.75">
-      <c r="C2105" s="2"/>
-    </row>
-    <row r="2106" spans="3:3" ht="12.75">
-      <c r="C2106" s="2"/>
-    </row>
-    <row r="2107" spans="3:3" ht="12.75">
-      <c r="C2107" s="2"/>
-    </row>
-    <row r="2108" spans="3:3" ht="12.75">
-      <c r="C2108" s="2"/>
-    </row>
-    <row r="2109" spans="3:3" ht="12.75">
-      <c r="C2109" s="2"/>
-    </row>
-    <row r="2110" spans="3:3" ht="12.75">
-      <c r="C2110" s="2"/>
-    </row>
-    <row r="2111" spans="3:3" ht="12.75">
-      <c r="C2111" s="2"/>
-    </row>
-    <row r="2112" spans="3:3" ht="12.75">
-      <c r="C2112" s="2"/>
-    </row>
-    <row r="2113" spans="3:3" ht="12.75">
-      <c r="C2113" s="2"/>
-    </row>
-    <row r="2114" spans="3:3" ht="12.75">
-      <c r="C2114" s="2"/>
-    </row>
-    <row r="2115" spans="3:3" ht="12.75">
-      <c r="C2115" s="2"/>
-    </row>
-    <row r="2116" spans="3:3" ht="12.75">
-      <c r="C2116" s="2"/>
-    </row>
-    <row r="2117" spans="3:3" ht="12.75">
-      <c r="C2117" s="2"/>
-    </row>
-    <row r="2118" spans="3:3" ht="12.75">
-      <c r="C2118" s="2"/>
-    </row>
-    <row r="2119" spans="3:3" ht="12.75">
-      <c r="C2119" s="2"/>
-    </row>
-    <row r="2120" spans="3:3" ht="12.75">
-      <c r="C2120" s="2"/>
-    </row>
-    <row r="2121" spans="3:3" ht="12.75">
-      <c r="C2121" s="2"/>
-    </row>
-    <row r="2122" spans="3:3" ht="12.75">
-      <c r="C2122" s="2"/>
-    </row>
-    <row r="2123" spans="3:3" ht="12.75">
-      <c r="C2123" s="2"/>
-    </row>
-    <row r="2124" spans="3:3" ht="12.75">
-      <c r="C2124" s="2"/>
-    </row>
-    <row r="2125" spans="3:3" ht="12.75">
-      <c r="C2125" s="2"/>
-    </row>
-    <row r="2126" spans="3:3" ht="12.75">
-      <c r="C2126" s="2"/>
-    </row>
-    <row r="2127" spans="3:3" ht="12.75">
-      <c r="C2127" s="2"/>
-    </row>
-    <row r="2128" spans="3:3" ht="12.75">
-      <c r="C2128" s="2"/>
-    </row>
-    <row r="2129" spans="3:3" ht="12.75">
-      <c r="C2129" s="2"/>
-    </row>
-    <row r="2130" spans="3:3" ht="12.75">
-      <c r="C2130" s="2"/>
-    </row>
-    <row r="2131" spans="3:3" ht="12.75">
-      <c r="C2131" s="2"/>
-    </row>
-    <row r="2132" spans="3:3" ht="12.75">
-      <c r="C2132" s="2"/>
-    </row>
-    <row r="2133" spans="3:3" ht="12.75">
-      <c r="C2133" s="2"/>
-    </row>
-    <row r="2134" spans="3:3" ht="12.75">
-      <c r="C2134" s="2"/>
-    </row>
-    <row r="2135" spans="3:3" ht="12.75">
-      <c r="C2135" s="2"/>
-    </row>
-    <row r="2136" spans="3:3" ht="12.75">
-      <c r="C2136" s="2"/>
-    </row>
-    <row r="2137" spans="3:3" ht="12.75">
-      <c r="C2137" s="2"/>
-    </row>
-    <row r="2138" spans="3:3" ht="12.75">
-      <c r="C2138" s="2"/>
-    </row>
-    <row r="2139" spans="3:3" ht="12.75">
-      <c r="C2139" s="2"/>
-    </row>
-    <row r="2140" spans="3:3" ht="12.75">
-      <c r="C2140" s="2"/>
-    </row>
-    <row r="2141" spans="3:3" ht="12.75">
-      <c r="C2141" s="2"/>
-    </row>
-    <row r="2142" spans="3:3" ht="12.75">
-      <c r="C2142" s="2"/>
-    </row>
-    <row r="2143" spans="3:3" ht="12.75">
-      <c r="C2143" s="2"/>
-    </row>
-    <row r="2144" spans="3:3" ht="12.75">
-      <c r="C2144" s="2"/>
-    </row>
-    <row r="2145" spans="3:3" ht="12.75">
-      <c r="C2145" s="2"/>
-    </row>
-    <row r="2146" spans="3:3" ht="12.75">
-      <c r="C2146" s="2"/>
-    </row>
-    <row r="2147" spans="3:3" ht="12.75">
-      <c r="C2147" s="2"/>
-    </row>
-    <row r="2148" spans="3:3" ht="12.75">
-      <c r="C2148" s="2"/>
-    </row>
-    <row r="2149" spans="3:3" ht="12.75">
-      <c r="C2149" s="2"/>
-    </row>
-    <row r="2150" spans="3:3" ht="12.75">
-      <c r="C2150" s="2"/>
-    </row>
-    <row r="2151" spans="3:3" ht="12.75">
-      <c r="C2151" s="2"/>
-    </row>
-    <row r="2152" spans="3:3" ht="12.75">
-      <c r="C2152" s="2"/>
-    </row>
-    <row r="2153" spans="3:3" ht="12.75">
-      <c r="C2153" s="2"/>
-    </row>
-    <row r="2154" spans="3:3" ht="12.75">
-      <c r="C2154" s="2"/>
-    </row>
-    <row r="2155" spans="3:3" ht="12.75">
-      <c r="C2155" s="2"/>
-    </row>
-    <row r="2156" spans="3:3" ht="12.75">
-      <c r="C2156" s="2"/>
-    </row>
-    <row r="2157" spans="3:3" ht="12.75">
-      <c r="C2157" s="2"/>
-    </row>
-    <row r="2158" spans="3:3" ht="12.75">
-      <c r="C2158" s="2"/>
-    </row>
-    <row r="2159" spans="3:3" ht="12.75">
-      <c r="C2159" s="2"/>
-    </row>
-    <row r="2160" spans="3:3" ht="12.75">
-      <c r="C2160" s="2"/>
-    </row>
-    <row r="2161" spans="3:3" ht="12.75">
-      <c r="C2161" s="2"/>
-    </row>
-    <row r="2162" spans="3:3" ht="12.75">
-      <c r="C2162" s="2"/>
-    </row>
-    <row r="2163" spans="3:3" ht="12.75">
-      <c r="C2163" s="2"/>
-    </row>
-    <row r="2164" spans="3:3" ht="12.75">
-      <c r="C2164" s="2"/>
-    </row>
-    <row r="2165" spans="3:3" ht="12.75">
-      <c r="C2165" s="2"/>
-    </row>
-    <row r="2166" spans="3:3" ht="12.75">
-      <c r="C2166" s="2"/>
-    </row>
-    <row r="2167" spans="3:3" ht="12.75">
-      <c r="C2167" s="2"/>
-    </row>
-    <row r="2168" spans="3:3" ht="12.75">
-      <c r="C2168" s="2"/>
-    </row>
-    <row r="2169" spans="3:3" ht="12.75">
-      <c r="C2169" s="2"/>
-    </row>
-    <row r="2170" spans="3:3" ht="12.75">
-      <c r="C2170" s="2"/>
-    </row>
-    <row r="2171" spans="3:3" ht="12.75">
-      <c r="C2171" s="2"/>
-    </row>
-    <row r="2172" spans="3:3" ht="12.75">
-      <c r="C2172" s="2"/>
-    </row>
-    <row r="2173" spans="3:3" ht="12.75">
-      <c r="C2173" s="2"/>
-    </row>
-    <row r="2174" spans="3:3" ht="12.75">
-      <c r="C2174" s="2"/>
-    </row>
-    <row r="2175" spans="3:3" ht="12.75">
-      <c r="C2175" s="2"/>
-    </row>
-    <row r="2176" spans="3:3" ht="12.75">
-      <c r="C2176" s="2"/>
-    </row>
-    <row r="2177" spans="3:3" ht="12.75">
-      <c r="C2177" s="2"/>
-    </row>
-    <row r="2178" spans="3:3" ht="12.75">
-      <c r="C2178" s="2"/>
-    </row>
-    <row r="2179" spans="3:3" ht="12.75">
-      <c r="C2179" s="2"/>
-    </row>
-    <row r="2180" spans="3:3" ht="12.75">
-      <c r="C2180" s="2"/>
-    </row>
-    <row r="2181" spans="3:3" ht="12.75">
-      <c r="C2181" s="2"/>
-    </row>
-    <row r="2182" spans="3:3" ht="12.75">
-      <c r="C2182" s="2"/>
-    </row>
-    <row r="2183" spans="3:3" ht="12.75">
-      <c r="C2183" s="2"/>
-    </row>
-    <row r="2184" spans="3:3" ht="12.75">
-      <c r="C2184" s="2"/>
-    </row>
-    <row r="2185" spans="3:3" ht="12.75">
-      <c r="C2185" s="2"/>
-    </row>
-    <row r="2186" spans="3:3" ht="12.75">
-      <c r="C2186" s="2"/>
-    </row>
-    <row r="2187" spans="3:3" ht="12.75">
-      <c r="C2187" s="2"/>
-    </row>
-    <row r="2188" spans="3:3" ht="12.75">
-      <c r="C2188" s="2"/>
-    </row>
-    <row r="2189" spans="3:3" ht="12.75">
-      <c r="C2189" s="2"/>
-    </row>
-    <row r="2190" spans="3:3" ht="12.75">
-      <c r="C2190" s="2"/>
-    </row>
-    <row r="2191" spans="3:3" ht="12.75">
-      <c r="C2191" s="2"/>
-    </row>
-    <row r="2192" spans="3:3" ht="12.75">
-      <c r="C2192" s="2"/>
-    </row>
-    <row r="2193" spans="3:3" ht="12.75">
-      <c r="C2193" s="2"/>
-    </row>
-    <row r="2194" spans="3:3" ht="12.75">
-      <c r="C2194" s="2"/>
-    </row>
-    <row r="2195" spans="3:3" ht="12.75">
-      <c r="C2195" s="2"/>
-    </row>
-    <row r="2196" spans="3:3" ht="12.75">
-      <c r="C2196" s="2"/>
-    </row>
-    <row r="2197" spans="3:3" ht="12.75">
-      <c r="C2197" s="2"/>
-    </row>
-    <row r="2198" spans="3:3" ht="12.75">
-      <c r="C2198" s="2"/>
-    </row>
-    <row r="2199" spans="3:3" ht="12.75">
-      <c r="C2199" s="2"/>
-    </row>
-    <row r="2200" spans="3:3" ht="12.75">
-      <c r="C2200" s="2"/>
-    </row>
-    <row r="2201" spans="3:3" ht="12.75">
-      <c r="C2201" s="2"/>
-    </row>
-    <row r="2202" spans="3:3" ht="12.75">
-      <c r="C2202" s="2"/>
-    </row>
-    <row r="2203" spans="3:3" ht="12.75">
-      <c r="C2203" s="2"/>
-    </row>
-    <row r="2204" spans="3:3" ht="12.75">
-      <c r="C2204" s="2"/>
-    </row>
-    <row r="2205" spans="3:3" ht="12.75">
-      <c r="C2205" s="2"/>
-    </row>
-    <row r="2206" spans="3:3" ht="12.75">
-      <c r="C2206" s="2"/>
-    </row>
-    <row r="2207" spans="3:3" ht="12.75">
-      <c r="C2207" s="2"/>
-    </row>
-    <row r="2208" spans="3:3" ht="12.75">
-      <c r="C2208" s="2"/>
-    </row>
-    <row r="2209" spans="3:3" ht="12.75">
-      <c r="C2209" s="2"/>
-    </row>
-    <row r="2210" spans="3:3" ht="12.75">
-      <c r="C2210" s="2"/>
-    </row>
-    <row r="2211" spans="3:3" ht="12.75">
-      <c r="C2211" s="2"/>
-    </row>
-    <row r="2212" spans="3:3" ht="12.75">
-      <c r="C2212" s="2"/>
-    </row>
-    <row r="2213" spans="3:3" ht="12.75">
-      <c r="C2213" s="2"/>
-    </row>
-    <row r="2214" spans="3:3" ht="12.75">
-      <c r="C2214" s="2"/>
-    </row>
-    <row r="2215" spans="3:3" ht="12.75">
-      <c r="C2215" s="2"/>
-    </row>
-    <row r="2216" spans="3:3" ht="12.75">
-      <c r="C2216" s="2"/>
-    </row>
-    <row r="2217" spans="3:3" ht="12.75">
-      <c r="C2217" s="2"/>
-    </row>
-    <row r="2218" spans="3:3" ht="12.75">
-      <c r="C2218" s="2"/>
-    </row>
-    <row r="2219" spans="3:3" ht="12.75">
-      <c r="C2219" s="2"/>
-    </row>
-    <row r="2220" spans="3:3" ht="12.75">
-      <c r="C2220" s="2"/>
-    </row>
-    <row r="2221" spans="3:3" ht="12.75">
-      <c r="C2221" s="2"/>
-    </row>
-    <row r="2222" spans="3:3" ht="12.75">
-      <c r="C2222" s="2"/>
-    </row>
-    <row r="2223" spans="3:3" ht="12.75">
-      <c r="C2223" s="2"/>
-    </row>
-    <row r="2224" spans="3:3" ht="12.75">
-      <c r="C2224" s="2"/>
-    </row>
-    <row r="2225" spans="3:3" ht="12.75">
-      <c r="C2225" s="2"/>
-    </row>
-    <row r="2226" spans="3:3" ht="12.75">
-      <c r="C2226" s="2"/>
-    </row>
-    <row r="2227" spans="3:3" ht="12.75">
-      <c r="C2227" s="2"/>
-    </row>
-    <row r="2228" spans="3:3" ht="12.75">
-      <c r="C2228" s="2"/>
-    </row>
-    <row r="2229" spans="3:3" ht="12.75">
-      <c r="C2229" s="2"/>
-    </row>
-    <row r="2230" spans="3:3" ht="12.75">
-      <c r="C2230" s="2"/>
-    </row>
-    <row r="2231" spans="3:3" ht="12.75">
-      <c r="C2231" s="2"/>
-    </row>
-    <row r="2232" spans="3:3" ht="12.75">
-      <c r="C2232" s="2"/>
-    </row>
-    <row r="2233" spans="3:3" ht="12.75">
-      <c r="C2233" s="2"/>
-    </row>
-    <row r="2234" spans="3:3" ht="12.75">
-      <c r="C2234" s="2"/>
-    </row>
-    <row r="2235" spans="3:3" ht="12.75">
-      <c r="C2235" s="2"/>
-    </row>
-    <row r="2236" spans="3:3" ht="12.75">
-      <c r="C2236" s="2"/>
-    </row>
-    <row r="2237" spans="3:3" ht="12.75">
-      <c r="C2237" s="2"/>
-    </row>
-    <row r="2238" spans="3:3" ht="12.75">
-      <c r="C2238" s="2"/>
-    </row>
-    <row r="2239" spans="3:3" ht="12.75">
-      <c r="C2239" s="2"/>
-    </row>
-    <row r="2240" spans="3:3" ht="12.75">
-      <c r="C2240" s="2"/>
-    </row>
-    <row r="2241" spans="3:3" ht="12.75">
-      <c r="C2241" s="2"/>
-    </row>
-    <row r="2242" spans="3:3" ht="12.75">
-      <c r="C2242" s="2"/>
-    </row>
-    <row r="2243" spans="3:3" ht="12.75">
-      <c r="C2243" s="2"/>
-    </row>
-    <row r="2244" spans="3:3" ht="12.75">
-      <c r="C2244" s="2"/>
-    </row>
-    <row r="2245" spans="3:3" ht="12.75">
-      <c r="C2245" s="2"/>
-    </row>
-    <row r="2246" spans="3:3" ht="12.75">
-      <c r="C2246" s="2"/>
-    </row>
-    <row r="2247" spans="3:3" ht="12.75">
-      <c r="C2247" s="2"/>
-    </row>
-    <row r="2248" spans="3:3" ht="12.75">
-      <c r="C2248" s="2"/>
-    </row>
-    <row r="2249" spans="3:3" ht="12.75">
-      <c r="C2249" s="2"/>
-    </row>
-    <row r="2250" spans="3:3" ht="12.75">
-      <c r="C2250" s="2"/>
-    </row>
-    <row r="2251" spans="3:3" ht="12.75">
-      <c r="C2251" s="2"/>
-    </row>
-    <row r="2252" spans="3:3" ht="12.75">
-      <c r="C2252" s="2"/>
-    </row>
-    <row r="2253" spans="3:3" ht="12.75">
-      <c r="C2253" s="2"/>
-    </row>
-    <row r="2254" spans="3:3" ht="12.75">
-      <c r="C2254" s="2"/>
-    </row>
-    <row r="2255" spans="3:3" ht="12.75">
-      <c r="C2255" s="2"/>
-    </row>
-    <row r="2256" spans="3:3" ht="12.75">
-      <c r="C2256" s="2"/>
-    </row>
-    <row r="2257" spans="3:3" ht="12.75">
-      <c r="C2257" s="2"/>
-    </row>
-    <row r="2258" spans="3:3" ht="12.75">
-      <c r="C2258" s="2"/>
-    </row>
-    <row r="2259" spans="3:3" ht="12.75">
-      <c r="C2259" s="2"/>
-    </row>
-    <row r="2260" spans="3:3" ht="12.75">
-      <c r="C2260" s="2"/>
-    </row>
-    <row r="2261" spans="3:3" ht="12.75">
-      <c r="C2261" s="2"/>
-    </row>
-    <row r="2262" spans="3:3" ht="12.75">
-      <c r="C2262" s="2"/>
-    </row>
-    <row r="2263" spans="3:3" ht="12.75">
-      <c r="C2263" s="2"/>
-    </row>
-    <row r="2264" spans="3:3" ht="12.75">
-      <c r="C2264" s="2"/>
-    </row>
-    <row r="2265" spans="3:3" ht="12.75">
-      <c r="C2265" s="2"/>
-    </row>
-    <row r="2266" spans="3:3" ht="12.75">
-      <c r="C2266" s="2"/>
-    </row>
-    <row r="2267" spans="3:3" ht="12.75">
-      <c r="C2267" s="2"/>
-    </row>
-    <row r="2268" spans="3:3" ht="12.75">
-      <c r="C2268" s="2"/>
-    </row>
-    <row r="2269" spans="3:3" ht="12.75">
-      <c r="C2269" s="2"/>
-    </row>
-    <row r="2270" spans="3:3" ht="12.75">
-      <c r="C2270" s="2"/>
-    </row>
-    <row r="2271" spans="3:3" ht="12.75">
-      <c r="C2271" s="2"/>
-    </row>
-    <row r="2272" spans="3:3" ht="12.75">
-      <c r="C2272" s="2"/>
-    </row>
-    <row r="2273" spans="3:3" ht="12.75">
-      <c r="C2273" s="2"/>
-    </row>
-    <row r="2274" spans="3:3" ht="12.75">
-      <c r="C2274" s="2"/>
-    </row>
-    <row r="2275" spans="3:3" ht="12.75">
-      <c r="C2275" s="2"/>
-    </row>
-    <row r="2276" spans="3:3" ht="12.75">
-      <c r="C2276" s="2"/>
-    </row>
-    <row r="2277" spans="3:3" ht="12.75">
-      <c r="C2277" s="2"/>
-    </row>
-    <row r="2278" spans="3:3" ht="12.75">
-      <c r="C2278" s="2"/>
-    </row>
-    <row r="2279" spans="3:3" ht="12.75">
-      <c r="C2279" s="2"/>
-    </row>
-    <row r="2280" spans="3:3" ht="12.75">
-      <c r="C2280" s="2"/>
-    </row>
-    <row r="2281" spans="3:3" ht="12.75">
-      <c r="C2281" s="2"/>
-    </row>
-    <row r="2282" spans="3:3" ht="12.75">
-      <c r="C2282" s="2"/>
-    </row>
-    <row r="2283" spans="3:3" ht="12.75">
-      <c r="C2283" s="2"/>
-    </row>
-    <row r="2284" spans="3:3" ht="12.75">
-      <c r="C2284" s="2"/>
-    </row>
-    <row r="2285" spans="3:3" ht="12.75">
-      <c r="C2285" s="2"/>
-    </row>
-    <row r="2286" spans="3:3" ht="12.75">
-      <c r="C2286" s="2"/>
-    </row>
-    <row r="2287" spans="3:3" ht="12.75">
-      <c r="C2287" s="2"/>
-    </row>
-    <row r="2288" spans="3:3" ht="12.75">
-      <c r="C2288" s="2"/>
-    </row>
-    <row r="2289" spans="3:3" ht="12.75">
-      <c r="C2289" s="2"/>
-    </row>
-    <row r="2290" spans="3:3" ht="12.75">
-      <c r="C2290" s="2"/>
-    </row>
-    <row r="2291" spans="3:3" ht="12.75">
-      <c r="C2291" s="2"/>
-    </row>
-    <row r="2292" spans="3:3" ht="12.75">
-      <c r="C2292" s="2"/>
-    </row>
-    <row r="2293" spans="3:3" ht="12.75">
-      <c r="C2293" s="2"/>
-    </row>
-    <row r="2294" spans="3:3" ht="12.75">
-      <c r="C2294" s="2"/>
-    </row>
-    <row r="2295" spans="3:3" ht="12.75">
-      <c r="C2295" s="2"/>
-    </row>
-    <row r="2296" spans="3:3" ht="12.75">
-      <c r="C2296" s="2"/>
-    </row>
-    <row r="2297" spans="3:3" ht="12.75">
-      <c r="C2297" s="2"/>
-    </row>
-    <row r="2298" spans="3:3" ht="12.75">
-      <c r="C2298" s="2"/>
-    </row>
-    <row r="2299" spans="3:3" ht="12.75">
-      <c r="C2299" s="2"/>
-    </row>
-    <row r="2300" spans="3:3" ht="12.75">
-      <c r="C2300" s="2"/>
-    </row>
-    <row r="2301" spans="3:3" ht="12.75">
-      <c r="C2301" s="2"/>
-    </row>
-    <row r="2302" spans="3:3" ht="12.75">
-      <c r="C2302" s="2"/>
-    </row>
-    <row r="2303" spans="3:3" ht="12.75">
-      <c r="C2303" s="2"/>
-    </row>
-    <row r="2304" spans="3:3" ht="12.75">
-      <c r="C2304" s="2"/>
-    </row>
-    <row r="2305" spans="3:3" ht="12.75">
-      <c r="C2305" s="2"/>
-    </row>
-    <row r="2306" spans="3:3" ht="12.75">
-      <c r="C2306" s="2"/>
-    </row>
-    <row r="2307" spans="3:3" ht="12.75">
-      <c r="C2307" s="2"/>
-    </row>
-    <row r="2308" spans="3:3" ht="12.75">
-      <c r="C2308" s="2"/>
-    </row>
-    <row r="2309" spans="3:3" ht="12.75">
-      <c r="C2309" s="2"/>
-    </row>
-    <row r="2310" spans="3:3" ht="12.75">
-      <c r="C2310" s="2"/>
-    </row>
-    <row r="2311" spans="3:3" ht="12.75">
-      <c r="C2311" s="2"/>
-    </row>
-    <row r="2312" spans="3:3" ht="12.75">
-      <c r="C2312" s="2"/>
-    </row>
-    <row r="2313" spans="3:3" ht="12.75">
-      <c r="C2313" s="2"/>
-    </row>
-    <row r="2314" spans="3:3" ht="12.75">
-      <c r="C2314" s="2"/>
-    </row>
-    <row r="2315" spans="3:3" ht="12.75">
-      <c r="C2315" s="2"/>
-    </row>
-    <row r="2316" spans="3:3" ht="12.75">
-      <c r="C2316" s="2"/>
-    </row>
-    <row r="2317" spans="3:3" ht="12.75">
-      <c r="C2317" s="2"/>
-    </row>
-    <row r="2318" spans="3:3" ht="12.75">
-      <c r="C2318" s="2"/>
-    </row>
-    <row r="2319" spans="3:3" ht="12.75">
-      <c r="C2319" s="2"/>
-    </row>
-    <row r="2320" spans="3:3" ht="12.75">
-      <c r="C2320" s="2"/>
-    </row>
-    <row r="2321" spans="3:3" ht="12.75">
-      <c r="C2321" s="2"/>
-    </row>
-    <row r="2322" spans="3:3" ht="12.75">
-      <c r="C2322" s="2"/>
-    </row>
-    <row r="2323" spans="3:3" ht="12.75">
-      <c r="C2323" s="2"/>
-    </row>
-    <row r="2324" spans="3:3" ht="12.75">
-      <c r="C2324" s="2"/>
-    </row>
-    <row r="2325" spans="3:3" ht="12.75">
-      <c r="C2325" s="2"/>
-    </row>
-    <row r="2326" spans="3:3" ht="12.75">
-      <c r="C2326" s="2"/>
-    </row>
-    <row r="2327" spans="3:3" ht="12.75">
-      <c r="C2327" s="2"/>
-    </row>
-    <row r="2328" spans="3:3" ht="12.75">
-      <c r="C2328" s="2"/>
-    </row>
-    <row r="2329" spans="3:3" ht="12.75">
-      <c r="C2329" s="2"/>
-    </row>
-    <row r="2330" spans="3:3" ht="12.75">
-      <c r="C2330" s="2"/>
-    </row>
-    <row r="2331" spans="3:3" ht="12.75">
-      <c r="C2331" s="2"/>
-    </row>
-    <row r="2332" spans="3:3" ht="12.75">
-      <c r="C2332" s="2"/>
-    </row>
-    <row r="2333" spans="3:3" ht="12.75">
-      <c r="C2333" s="2"/>
-    </row>
-    <row r="2334" spans="3:3" ht="12.75">
-      <c r="C2334" s="2"/>
-    </row>
-    <row r="2335" spans="3:3" ht="12.75">
-      <c r="C2335" s="2"/>
-    </row>
-    <row r="2336" spans="3:3" ht="12.75">
-      <c r="C2336" s="2"/>
-    </row>
-    <row r="2337" spans="3:3" ht="12.75">
-      <c r="C2337" s="2"/>
-    </row>
-    <row r="2338" spans="3:3" ht="12.75">
-      <c r="C2338" s="2"/>
-    </row>
-    <row r="2339" spans="3:3" ht="12.75">
-      <c r="C2339" s="2"/>
-    </row>
-    <row r="2340" spans="3:3" ht="12.75">
-      <c r="C2340" s="2"/>
-    </row>
-    <row r="2341" spans="3:3" ht="12.75">
-      <c r="C2341" s="2"/>
-    </row>
-    <row r="2342" spans="3:3" ht="12.75">
-      <c r="C2342" s="2"/>
-    </row>
-    <row r="2343" spans="3:3" ht="12.75">
-      <c r="C2343" s="2"/>
-    </row>
-    <row r="2344" spans="3:3" ht="12.75">
-      <c r="C2344" s="2"/>
-    </row>
-    <row r="2345" spans="3:3" ht="12.75">
-      <c r="C2345" s="2"/>
-    </row>
-    <row r="2346" spans="3:3" ht="12.75">
-      <c r="C2346" s="2"/>
-    </row>
-    <row r="2347" spans="3:3" ht="12.75">
-      <c r="C2347" s="2"/>
-    </row>
-    <row r="2348" spans="3:3" ht="12.75">
-      <c r="C2348" s="2"/>
-    </row>
-    <row r="2349" spans="3:3" ht="12.75">
-      <c r="C2349" s="2"/>
-    </row>
-    <row r="2350" spans="3:3" ht="12.75">
-      <c r="C2350" s="2"/>
-    </row>
-    <row r="2351" spans="3:3" ht="12.75">
-      <c r="C2351" s="2"/>
-    </row>
-    <row r="2352" spans="3:3" ht="12.75">
-      <c r="C2352" s="2"/>
-    </row>
-    <row r="2353" spans="3:3" ht="12.75">
-      <c r="C2353" s="2"/>
-    </row>
-    <row r="2354" spans="3:3" ht="12.75">
-      <c r="C2354" s="2"/>
-    </row>
-    <row r="2355" spans="3:3" ht="12.75">
-      <c r="C2355" s="2"/>
-    </row>
-    <row r="2356" spans="3:3" ht="12.75">
-      <c r="C2356" s="2"/>
-    </row>
-    <row r="2357" spans="3:3" ht="12.75">
-      <c r="C2357" s="2"/>
-    </row>
-    <row r="2358" spans="3:3" ht="12.75">
-      <c r="C2358" s="2"/>
-    </row>
-    <row r="2359" spans="3:3" ht="12.75">
-      <c r="C2359" s="2"/>
-    </row>
-    <row r="2360" spans="3:3" ht="12.75">
-      <c r="C2360" s="2"/>
-    </row>
-    <row r="2361" spans="3:3" ht="12.75">
-      <c r="C2361" s="2"/>
-    </row>
-    <row r="2362" spans="3:3" ht="12.75">
-      <c r="C2362" s="2"/>
-    </row>
-    <row r="2363" spans="3:3" ht="12.75">
-      <c r="C2363" s="2"/>
-    </row>
-    <row r="2364" spans="3:3" ht="12.75">
-      <c r="C2364" s="2"/>
-    </row>
-    <row r="2365" spans="3:3" ht="12.75">
-      <c r="C2365" s="2"/>
-    </row>
-    <row r="2366" spans="3:3" ht="12.75">
-      <c r="C2366" s="2"/>
-    </row>
-    <row r="2367" spans="3:3" ht="12.75">
-      <c r="C2367" s="2"/>
-    </row>
-    <row r="2368" spans="3:3" ht="12.75">
-      <c r="C2368" s="2"/>
-    </row>
-    <row r="2369" spans="3:3" ht="12.75">
-      <c r="C2369" s="2"/>
-    </row>
-    <row r="2370" spans="3:3" ht="12.75">
-      <c r="C2370" s="2"/>
-    </row>
-    <row r="2371" spans="3:3" ht="12.75">
-      <c r="C2371" s="2"/>
-    </row>
-    <row r="2372" spans="3:3" ht="12.75">
-      <c r="C2372" s="2"/>
-    </row>
-    <row r="2373" spans="3:3" ht="12.75">
-      <c r="C2373" s="2"/>
-    </row>
-    <row r="2374" spans="3:3" ht="12.75">
-      <c r="C2374" s="2"/>
-    </row>
-    <row r="2375" spans="3:3" ht="12.75">
-      <c r="C2375" s="2"/>
-    </row>
-    <row r="2376" spans="3:3" ht="12.75">
-      <c r="C2376" s="2"/>
-    </row>
-    <row r="2377" spans="3:3" ht="12.75">
-      <c r="C2377" s="2"/>
-    </row>
-    <row r="2378" spans="3:3" ht="12.75">
-      <c r="C2378" s="2"/>
-    </row>
-    <row r="2379" spans="3:3" ht="12.75">
-      <c r="C2379" s="2"/>
-    </row>
-    <row r="2380" spans="3:3" ht="12.75">
-      <c r="C2380" s="2"/>
-    </row>
-    <row r="2381" spans="3:3" ht="12.75">
-      <c r="C2381" s="2"/>
-    </row>
-    <row r="2382" spans="3:3" ht="12.75">
-      <c r="C2382" s="2"/>
-    </row>
-    <row r="2383" spans="3:3" ht="12.75">
-      <c r="C2383" s="2"/>
-    </row>
-    <row r="2384" spans="3:3" ht="12.75">
-      <c r="C2384" s="2"/>
-    </row>
-    <row r="2385" spans="3:3" ht="12.75">
-      <c r="C2385" s="2"/>
-    </row>
-    <row r="2386" spans="3:3" ht="12.75">
-      <c r="C2386" s="2"/>
-    </row>
-    <row r="2387" spans="3:3" ht="12.75">
-      <c r="C2387" s="2"/>
-    </row>
-    <row r="2388" spans="3:3" ht="12.75">
-      <c r="C2388" s="2"/>
-    </row>
-    <row r="2389" spans="3:3" ht="12.75">
-      <c r="C2389" s="2"/>
-    </row>
-    <row r="2390" spans="3:3" ht="12.75">
-      <c r="C2390" s="2"/>
-    </row>
-    <row r="2391" spans="3:3" ht="12.75">
-      <c r="C2391" s="2"/>
-    </row>
-    <row r="2392" spans="3:3" ht="12.75">
-      <c r="C2392" s="2"/>
-    </row>
-    <row r="2393" spans="3:3" ht="12.75">
-      <c r="C2393" s="2"/>
-    </row>
-    <row r="2394" spans="3:3" ht="12.75">
-      <c r="C2394" s="2"/>
-    </row>
-    <row r="2395" spans="3:3" ht="12.75">
-      <c r="C2395" s="2"/>
-    </row>
-    <row r="2396" spans="3:3" ht="12.75">
-      <c r="C2396" s="2"/>
-    </row>
-    <row r="2397" spans="3:3" ht="12.75">
-      <c r="C2397" s="2"/>
-    </row>
-    <row r="2398" spans="3:3" ht="12.75">
-      <c r="C2398" s="2"/>
-    </row>
-    <row r="2399" spans="3:3" ht="12.75">
-      <c r="C2399" s="2"/>
-    </row>
-    <row r="2400" spans="3:3" ht="12.75">
-      <c r="C2400" s="2"/>
-    </row>
-    <row r="2401" spans="1:3" ht="12.75">
-      <c r="C2401" s="2"/>
-    </row>
-    <row r="2402" spans="1:3" ht="12.75">
-      <c r="C2402" s="2"/>
-    </row>
-    <row r="2403" spans="1:3" ht="12.75">
-      <c r="C2403" s="2"/>
-    </row>
-    <row r="2404" spans="1:3" ht="12.75">
-      <c r="C2404" s="2"/>
-    </row>
-    <row r="2405" spans="1:3" ht="12.75">
-      <c r="C2405" s="2"/>
-    </row>
-    <row r="2406" spans="1:3" ht="12.75">
-      <c r="C2406" s="2"/>
-    </row>
-    <row r="2407" spans="1:3" ht="12.75">
-      <c r="C2407" s="2"/>
-    </row>
-    <row r="2408" spans="1:3" ht="12.75">
-      <c r="C2408" s="2"/>
-    </row>
-    <row r="2409" spans="1:3" ht="12.75">
-      <c r="C2409" s="2"/>
-    </row>
-    <row r="2410" spans="1:3" ht="12.75">
-      <c r="C2410" s="2"/>
-    </row>
-    <row r="2411" spans="1:3" ht="12.75">
-      <c r="C2411" s="2"/>
-    </row>
-    <row r="2412" spans="1:3" ht="12.75">
-      <c r="A2412" s="1"/>
-      <c r="B2412" s="1"/>
-      <c r="C2412" s="2"/>
-    </row>
-    <row r="2413" spans="1:3" ht="12.75">
-      <c r="A2413" s="1"/>
-      <c r="B2413" s="1"/>
-      <c r="C2413" s="2"/>
-    </row>
-    <row r="2414" spans="1:3" ht="12.75">
-      <c r="A2414" s="1"/>
-      <c r="B2414" s="1"/>
-      <c r="C2414" s="2"/>
-    </row>
-    <row r="2415" spans="1:3" ht="12.75">
-      <c r="A2415" s="1"/>
-      <c r="B2415" s="1"/>
-      <c r="C2415" s="2"/>
-    </row>
-    <row r="2416" spans="1:3" ht="12.75">
-      <c r="A2416" s="1"/>
-      <c r="B2416" s="1"/>
-      <c r="C2416" s="2"/>
-    </row>
-    <row r="2417" spans="1:3" ht="12.75">
-      <c r="A2417" s="1"/>
-      <c r="B2417" s="1"/>
-      <c r="C2417" s="2"/>
-    </row>
-    <row r="2418" spans="1:3" ht="12.75">
-      <c r="A2418" s="1"/>
-      <c r="B2418" s="1"/>
-      <c r="C2418" s="2"/>
-    </row>
-    <row r="2419" spans="1:3" ht="12.75">
-      <c r="A2419" s="1"/>
-      <c r="B2419" s="1"/>
-      <c r="C2419" s="2"/>
-    </row>
-    <row r="2420" spans="1:3" ht="12.75">
-      <c r="A2420" s="1"/>
-      <c r="B2420" s="1"/>
-      <c r="C2420" s="2"/>
-    </row>
-    <row r="2421" spans="1:3" ht="12.75">
-      <c r="A2421" s="1"/>
-      <c r="B2421" s="1"/>
-      <c r="C2421" s="2"/>
-    </row>
-    <row r="2422" spans="1:3" ht="12.75">
-      <c r="A2422" s="1"/>
-      <c r="B2422" s="1"/>
-      <c r="C2422" s="2"/>
-    </row>
-    <row r="2423" spans="1:3" ht="12.75">
-      <c r="A2423" s="1"/>
-      <c r="B2423" s="1"/>
-      <c r="C2423" s="2"/>
-    </row>
-    <row r="2424" spans="1:3" ht="12.75">
-      <c r="A2424" s="1"/>
-      <c r="B2424" s="1"/>
-      <c r="C2424" s="2"/>
-    </row>
-    <row r="2425" spans="1:3" ht="12.75">
-      <c r="A2425" s="1"/>
-      <c r="B2425" s="1"/>
-      <c r="C2425" s="2"/>
-    </row>
-    <row r="2426" spans="1:3" ht="12.75">
-      <c r="A2426" s="1"/>
-      <c r="B2426" s="1"/>
-      <c r="C2426" s="2"/>
-    </row>
-    <row r="2427" spans="1:3" ht="12.75">
-      <c r="A2427" s="1"/>
-      <c r="B2427" s="1"/>
-      <c r="C2427" s="2"/>
-    </row>
-    <row r="2428" spans="1:3" ht="12.75">
-      <c r="A2428" s="1"/>
-      <c r="B2428" s="1"/>
-      <c r="C2428" s="2"/>
-    </row>
-    <row r="2429" spans="1:3" ht="12.75">
-      <c r="A2429" s="1"/>
-      <c r="B2429" s="1"/>
-      <c r="C2429" s="2"/>
-    </row>
-    <row r="2430" spans="1:3" ht="12.75">
-      <c r="A2430" s="1"/>
-      <c r="B2430" s="1"/>
-      <c r="C2430" s="2"/>
-    </row>
-    <row r="2431" spans="1:3" ht="12.75">
-      <c r="A2431" s="1"/>
-      <c r="B2431" s="1"/>
-      <c r="C2431" s="2"/>
-    </row>
-    <row r="2432" spans="1:3" ht="12.75">
-      <c r="A2432" s="1"/>
-      <c r="B2432" s="1"/>
-      <c r="C2432" s="2"/>
-    </row>
-    <row r="2433" spans="1:3" ht="12.75">
-      <c r="A2433" s="1"/>
-      <c r="B2433" s="1"/>
-      <c r="C2433" s="2"/>
-    </row>
-    <row r="2434" spans="1:3" ht="12.75">
-      <c r="A2434" s="1"/>
-      <c r="B2434" s="1"/>
-      <c r="C2434" s="2"/>
-    </row>
-    <row r="2435" spans="1:3" ht="12.75">
-      <c r="A2435" s="1"/>
-      <c r="B2435" s="1"/>
-      <c r="C2435" s="2"/>
-    </row>
-    <row r="2436" spans="1:3" ht="12.75">
-      <c r="A2436" s="1"/>
-      <c r="B2436" s="1"/>
-      <c r="C2436" s="2"/>
-    </row>
-    <row r="2437" spans="1:3" ht="12.75">
-      <c r="A2437" s="1"/>
-      <c r="B2437" s="1"/>
-      <c r="C2437" s="2"/>
-    </row>
-    <row r="2438" spans="1:3" ht="12.75">
-      <c r="A2438" s="1"/>
-      <c r="B2438" s="1"/>
-      <c r="C2438" s="2"/>
-    </row>
-    <row r="2439" spans="1:3" ht="12.75">
-      <c r="A2439" s="1"/>
-      <c r="B2439" s="1"/>
-      <c r="C2439" s="2"/>
-    </row>
-    <row r="2440" spans="1:3" ht="12.75">
-      <c r="A2440" s="1"/>
-      <c r="B2440" s="1"/>
-      <c r="C2440" s="2"/>
-    </row>
-    <row r="2441" spans="1:3" ht="12.75">
-      <c r="A2441" s="1"/>
-      <c r="B2441" s="1"/>
-      <c r="C2441" s="2"/>
-    </row>
-    <row r="2442" spans="1:3" ht="12.75">
-      <c r="A2442" s="1"/>
-      <c r="B2442" s="1"/>
-      <c r="C2442" s="2"/>
-    </row>
-    <row r="2443" spans="1:3" ht="12.75">
-      <c r="A2443" s="1"/>
-      <c r="B2443" s="1"/>
-      <c r="C2443" s="2"/>
-    </row>
-    <row r="2444" spans="1:3" ht="12.75">
-      <c r="A2444" s="1"/>
-      <c r="B2444" s="1"/>
-      <c r="C2444" s="2"/>
-    </row>
-    <row r="2445" spans="1:3" ht="12.75">
-      <c r="A2445" s="1"/>
-      <c r="B2445" s="1"/>
-      <c r="C2445" s="2"/>
-    </row>
-    <row r="2446" spans="1:3" ht="12.75">
-      <c r="A2446" s="1"/>
-      <c r="B2446" s="1"/>
-      <c r="C2446" s="2"/>
-    </row>
-    <row r="2447" spans="1:3" ht="12.75">
-      <c r="A2447" s="1"/>
-      <c r="B2447" s="1"/>
-      <c r="C2447" s="2"/>
-    </row>
-    <row r="2448" spans="1:3" ht="12.75">
-      <c r="A2448" s="1"/>
-      <c r="B2448" s="1"/>
-      <c r="C2448" s="2"/>
-    </row>
-    <row r="2449" spans="1:3" ht="12.75">
-      <c r="A2449" s="1"/>
-      <c r="B2449" s="1"/>
-      <c r="C2449" s="2"/>
-    </row>
-    <row r="2450" spans="1:3" ht="12.75">
-      <c r="A2450" s="1"/>
-      <c r="B2450" s="1"/>
-      <c r="C2450" s="2"/>
-    </row>
-    <row r="2451" spans="1:3" ht="12.75">
-      <c r="A2451" s="1"/>
-      <c r="B2451" s="1"/>
-      <c r="C2451" s="2"/>
-    </row>
-    <row r="2452" spans="1:3" ht="12.75">
-      <c r="A2452" s="1"/>
-      <c r="B2452" s="1"/>
-      <c r="C2452" s="2"/>
-    </row>
-    <row r="2453" spans="1:3" ht="12.75">
-      <c r="A2453" s="1"/>
-      <c r="B2453" s="1"/>
-      <c r="C2453" s="2"/>
-    </row>
-    <row r="2454" spans="1:3" ht="12.75">
-      <c r="A2454" s="1"/>
-      <c r="B2454" s="1"/>
-      <c r="C2454" s="2"/>
-    </row>
-    <row r="2455" spans="1:3" ht="12.75">
-      <c r="A2455" s="1"/>
-      <c r="B2455" s="1"/>
-      <c r="C2455" s="2"/>
-    </row>
-    <row r="2456" spans="1:3" ht="12.75">
-      <c r="A2456" s="1"/>
-      <c r="B2456" s="1"/>
-      <c r="C2456" s="2"/>
-    </row>
-    <row r="2457" spans="1:3" ht="12.75">
-      <c r="A2457" s="1"/>
-      <c r="B2457" s="1"/>
-      <c r="C2457" s="2"/>
-    </row>
-    <row r="2458" spans="1:3" ht="12.75">
-      <c r="A2458" s="1"/>
-      <c r="B2458" s="1"/>
-      <c r="C2458" s="2"/>
-    </row>
-    <row r="2459" spans="1:3" ht="12.75">
-      <c r="A2459" s="1"/>
-      <c r="B2459" s="1"/>
-      <c r="C2459" s="2"/>
-    </row>
-    <row r="2460" spans="1:3" ht="12.75">
-      <c r="A2460" s="1"/>
-      <c r="B2460" s="1"/>
-      <c r="C2460" s="2"/>
-    </row>
-    <row r="2461" spans="1:3" ht="12.75">
-      <c r="A2461" s="1"/>
-      <c r="B2461" s="1"/>
-      <c r="C2461" s="2"/>
-    </row>
-    <row r="2462" spans="1:3" ht="12.75">
-      <c r="A2462" s="1"/>
-      <c r="B2462" s="1"/>
-      <c r="C2462" s="2"/>
-    </row>
-    <row r="2463" spans="1:3" ht="12.75">
-      <c r="A2463" s="1"/>
-      <c r="B2463" s="1"/>
-      <c r="C2463" s="2"/>
-    </row>
-    <row r="2464" spans="1:3" ht="12.75">
-      <c r="A2464" s="1"/>
-      <c r="B2464" s="1"/>
-      <c r="C2464" s="2"/>
-    </row>
-    <row r="2465" spans="1:3" ht="12.75">
-      <c r="A2465" s="1"/>
-      <c r="B2465" s="1"/>
-      <c r="C2465" s="2"/>
-    </row>
-    <row r="2466" spans="1:3" ht="12.75">
-      <c r="A2466" s="1"/>
-      <c r="B2466" s="1"/>
-      <c r="C2466" s="2"/>
-    </row>
-    <row r="2467" spans="1:3" ht="12.75">
-      <c r="A2467" s="1"/>
-      <c r="B2467" s="1"/>
-      <c r="C2467" s="2"/>
-    </row>
-    <row r="2468" spans="1:3" ht="12.75">
-      <c r="A2468" s="1"/>
-      <c r="B2468" s="1"/>
-      <c r="C2468" s="2"/>
-    </row>
-    <row r="2469" spans="1:3" ht="12.75">
-      <c r="A2469" s="1"/>
-      <c r="B2469" s="1"/>
-      <c r="C2469" s="2"/>
-    </row>
-    <row r="2470" spans="1:3" ht="12.75">
-      <c r="A2470" s="1"/>
-      <c r="B2470" s="1"/>
-      <c r="C2470" s="2"/>
-    </row>
-    <row r="2471" spans="1:3" ht="12.75">
-      <c r="A2471" s="1"/>
-      <c r="B2471" s="1"/>
-      <c r="C2471" s="2"/>
-    </row>
-    <row r="2472" spans="1:3" ht="12.75">
-      <c r="A2472" s="1"/>
-      <c r="B2472" s="1"/>
-      <c r="C2472" s="2"/>
-    </row>
-    <row r="2473" spans="1:3" ht="12.75">
-      <c r="A2473" s="1"/>
-      <c r="B2473" s="1"/>
-      <c r="C2473" s="2"/>
-    </row>
-    <row r="2474" spans="1:3" ht="12.75">
-      <c r="A2474" s="1"/>
-      <c r="B2474" s="1"/>
-      <c r="C2474" s="2"/>
-    </row>
-    <row r="2475" spans="1:3" ht="12.75">
-      <c r="A2475" s="1"/>
-      <c r="B2475" s="1"/>
-      <c r="C2475" s="2"/>
-    </row>
-    <row r="2476" spans="1:3" ht="12.75">
-      <c r="A2476" s="1"/>
-      <c r="B2476" s="1"/>
-      <c r="C2476" s="2"/>
-    </row>
-    <row r="2477" spans="1:3" ht="12.75">
-      <c r="A2477" s="1"/>
-      <c r="B2477" s="1"/>
-      <c r="C2477" s="2"/>
-    </row>
-    <row r="2478" spans="1:3" ht="12.75">
-      <c r="A2478" s="1"/>
-      <c r="B2478" s="1"/>
-      <c r="C2478" s="2"/>
-    </row>
-    <row r="2479" spans="1:3" ht="12.75">
-      <c r="A2479" s="1"/>
-      <c r="B2479" s="1"/>
-      <c r="C2479" s="2"/>
-    </row>
-    <row r="2480" spans="1:3" ht="12.75">
-      <c r="A2480" s="1"/>
-      <c r="B2480" s="1"/>
-      <c r="C2480" s="2"/>
-    </row>
-    <row r="2481" spans="1:3" ht="12.75">
-      <c r="A2481" s="1"/>
-      <c r="B2481" s="1"/>
-      <c r="C2481" s="2"/>
-    </row>
-    <row r="2482" spans="1:3" ht="12.75">
-      <c r="A2482" s="1"/>
-      <c r="B2482" s="1"/>
-      <c r="C2482" s="2"/>
-    </row>
-    <row r="2483" spans="1:3" ht="12.75">
-      <c r="A2483" s="1"/>
-      <c r="B2483" s="1"/>
-      <c r="C2483" s="2"/>
-    </row>
-    <row r="2484" spans="1:3" ht="12.75">
-      <c r="A2484" s="1"/>
-      <c r="B2484" s="1"/>
-      <c r="C2484" s="2"/>
-    </row>
-    <row r="2485" spans="1:3" ht="12.75">
-      <c r="A2485" s="1"/>
-      <c r="B2485" s="1"/>
-      <c r="C2485" s="2"/>
-    </row>
-    <row r="2486" spans="1:3" ht="12.75">
-      <c r="A2486" s="1"/>
-      <c r="B2486" s="1"/>
-      <c r="C2486" s="2"/>
-    </row>
-    <row r="2487" spans="1:3" ht="12.75">
-      <c r="A2487" s="1"/>
-      <c r="B2487" s="1"/>
-      <c r="C2487" s="2"/>
-    </row>
-    <row r="2488" spans="1:3" ht="12.75">
-      <c r="A2488" s="1"/>
-      <c r="B2488" s="1"/>
-      <c r="C2488" s="2"/>
-    </row>
-    <row r="2489" spans="1:3" ht="12.75">
-      <c r="A2489" s="1"/>
-      <c r="B2489" s="1"/>
-      <c r="C2489" s="2"/>
-    </row>
-    <row r="2490" spans="1:3" ht="12.75">
-      <c r="A2490" s="1"/>
-      <c r="B2490" s="1"/>
-      <c r="C2490" s="2"/>
-    </row>
-    <row r="2491" spans="1:3" ht="12.75">
-      <c r="A2491" s="1"/>
-      <c r="B2491" s="1"/>
-      <c r="C2491" s="2"/>
-    </row>
-    <row r="2492" spans="1:3" ht="12.75">
-      <c r="A2492" s="1"/>
-      <c r="B2492" s="1"/>
-      <c r="C2492" s="2"/>
-    </row>
-    <row r="2493" spans="1:3" ht="12.75">
-      <c r="A2493" s="1"/>
-      <c r="B2493" s="1"/>
-      <c r="C2493" s="2"/>
-    </row>
-    <row r="2494" spans="1:3" ht="12.75">
-      <c r="A2494" s="1"/>
-      <c r="B2494" s="1"/>
-      <c r="C2494" s="2"/>
-    </row>
-    <row r="2495" spans="1:3" ht="12.75">
-      <c r="A2495" s="1"/>
-      <c r="B2495" s="1"/>
-      <c r="C2495" s="2"/>
-    </row>
-    <row r="2496" spans="1:3" ht="12.75">
-      <c r="A2496" s="1"/>
-      <c r="B2496" s="1"/>
-      <c r="C2496" s="2"/>
-    </row>
-    <row r="2497" spans="1:3" ht="12.75">
-      <c r="A2497" s="1"/>
-      <c r="B2497" s="1"/>
-      <c r="C2497" s="2"/>
-    </row>
-    <row r="2498" spans="1:3" ht="12.75">
-      <c r="A2498" s="1"/>
-      <c r="B2498" s="1"/>
-      <c r="C2498" s="2"/>
-    </row>
-    <row r="2499" spans="1:3" ht="12.75">
-      <c r="A2499" s="1"/>
-      <c r="B2499" s="1"/>
-      <c r="C2499" s="2"/>
-    </row>
-    <row r="2500" spans="1:3" ht="12.75">
-      <c r="A2500" s="1"/>
-      <c r="B2500" s="1"/>
-      <c r="C2500" s="2"/>
-    </row>
-    <row r="2501" spans="1:3" ht="12.75">
-      <c r="A2501" s="1"/>
-      <c r="B2501" s="1"/>
-      <c r="C2501" s="2"/>
-    </row>
-    <row r="2502" spans="1:3" ht="12.75">
-      <c r="A2502" s="1"/>
-      <c r="B2502" s="1"/>
-      <c r="C2502" s="2"/>
-    </row>
-    <row r="2503" spans="1:3" ht="12.75">
-      <c r="A2503" s="1"/>
-      <c r="B2503" s="1"/>
-      <c r="C2503" s="2"/>
-    </row>
-    <row r="2504" spans="1:3" ht="12.75">
-      <c r="A2504" s="1"/>
-      <c r="B2504" s="1"/>
-      <c r="C2504" s="2"/>
-    </row>
-    <row r="2505" spans="1:3" ht="12.75">
-      <c r="A2505" s="1"/>
-      <c r="B2505" s="1"/>
-      <c r="C2505" s="2"/>
-    </row>
-    <row r="2506" spans="1:3" ht="12.75">
-      <c r="A2506" s="1"/>
-      <c r="B2506" s="1"/>
-      <c r="C2506" s="2"/>
-    </row>
-    <row r="2507" spans="1:3" ht="12.75">
-      <c r="A2507" s="1"/>
-      <c r="B2507" s="1"/>
-      <c r="C2507" s="2"/>
-    </row>
-    <row r="2508" spans="1:3" ht="12.75">
-      <c r="A2508" s="1"/>
-      <c r="B2508" s="1"/>
-      <c r="C2508" s="2"/>
-    </row>
-    <row r="2509" spans="1:3" ht="12.75">
-      <c r="A2509" s="1"/>
-      <c r="B2509" s="1"/>
-      <c r="C2509" s="2"/>
-    </row>
-    <row r="2510" spans="1:3" ht="12.75">
-      <c r="A2510" s="1"/>
-      <c r="B2510" s="1"/>
-      <c r="C2510" s="2"/>
-    </row>
-    <row r="2511" spans="1:3" ht="12.75">
-      <c r="A2511" s="1"/>
-      <c r="B2511" s="1"/>
-      <c r="C2511" s="2"/>
-    </row>
-    <row r="2512" spans="1:3" ht="12.75">
-      <c r="A2512" s="1"/>
-      <c r="B2512" s="1"/>
-      <c r="C2512" s="2"/>
-    </row>
-    <row r="2513" spans="1:3" ht="12.75">
-      <c r="A2513" s="1"/>
-      <c r="B2513" s="1"/>
-      <c r="C2513" s="2"/>
-    </row>
-    <row r="2514" spans="1:3" ht="12.75">
-      <c r="A2514" s="1"/>
-      <c r="B2514" s="1"/>
-      <c r="C2514" s="2"/>
-    </row>
-    <row r="2515" spans="1:3" ht="12.75">
-      <c r="A2515" s="1"/>
-      <c r="B2515" s="1"/>
-      <c r="C2515" s="2"/>
-    </row>
-    <row r="2516" spans="1:3" ht="12.75">
-      <c r="A2516" s="1"/>
-      <c r="B2516" s="1"/>
-      <c r="C2516" s="2"/>
-    </row>
-    <row r="2517" spans="1:3" ht="12.75">
-      <c r="A2517" s="1"/>
-      <c r="B2517" s="1"/>
-      <c r="C2517" s="2"/>
-    </row>
-    <row r="2518" spans="1:3" ht="12.75">
-      <c r="A2518" s="1"/>
-      <c r="B2518" s="1"/>
-      <c r="C2518" s="2"/>
-    </row>
-    <row r="2519" spans="1:3" ht="12.75">
-      <c r="A2519" s="1"/>
-      <c r="B2519" s="1"/>
-      <c r="C2519" s="2"/>
-    </row>
-    <row r="2520" spans="1:3" ht="12.75">
-      <c r="A2520" s="1"/>
-      <c r="B2520" s="1"/>
-      <c r="C2520" s="2"/>
-    </row>
-    <row r="2521" spans="1:3" ht="12.75">
-      <c r="A2521" s="1"/>
-      <c r="B2521" s="1"/>
-      <c r="C2521" s="2"/>
-    </row>
-    <row r="2522" spans="1:3" ht="12.75">
-      <c r="A2522" s="1"/>
-      <c r="B2522" s="1"/>
-      <c r="C2522" s="2"/>
-    </row>
-    <row r="2523" spans="1:3" ht="12.75">
-      <c r="A2523" s="1"/>
-      <c r="B2523" s="1"/>
-      <c r="C2523" s="2"/>
-    </row>
-    <row r="2524" spans="1:3" ht="12.75">
-      <c r="A2524" s="1"/>
-      <c r="B2524" s="1"/>
-      <c r="C2524" s="2"/>
-    </row>
-    <row r="2525" spans="1:3" ht="12.75">
-      <c r="A2525" s="1"/>
-      <c r="B2525" s="1"/>
-      <c r="C2525" s="2"/>
-    </row>
-    <row r="2526" spans="1:3" ht="12.75">
-      <c r="A2526" s="1"/>
-      <c r="B2526" s="1"/>
-      <c r="C2526" s="2"/>
-    </row>
-    <row r="2527" spans="1:3" ht="12.75">
-      <c r="A2527" s="1"/>
-      <c r="B2527" s="1"/>
-      <c r="C2527" s="2"/>
-    </row>
-    <row r="2528" spans="1:3" ht="12.75">
-      <c r="A2528" s="1"/>
-      <c r="B2528" s="1"/>
-      <c r="C2528" s="2"/>
-    </row>
-    <row r="2529" spans="1:3" ht="12.75">
-      <c r="A2529" s="1"/>
-      <c r="B2529" s="1"/>
-      <c r="C2529" s="2"/>
-    </row>
-    <row r="2530" spans="1:3" ht="12.75">
-      <c r="A2530" s="1"/>
-      <c r="B2530" s="1"/>
-      <c r="C2530" s="2"/>
-    </row>
-    <row r="2531" spans="1:3" ht="12.75">
-      <c r="A2531" s="1"/>
-      <c r="B2531" s="1"/>
-      <c r="C2531" s="2"/>
-    </row>
-    <row r="2532" spans="1:3" ht="12.75">
-      <c r="A2532" s="1"/>
-      <c r="B2532" s="1"/>
-      <c r="C2532" s="2"/>
-    </row>
-    <row r="2533" spans="1:3" ht="12.75">
-      <c r="A2533" s="1"/>
-      <c r="B2533" s="1"/>
-      <c r="C2533" s="2"/>
-    </row>
-    <row r="2534" spans="1:3" ht="12.75">
-      <c r="A2534" s="1"/>
-      <c r="B2534" s="1"/>
-      <c r="C2534" s="2"/>
-    </row>
-    <row r="2535" spans="1:3" ht="12.75">
-      <c r="A2535" s="1"/>
-      <c r="B2535" s="1"/>
-      <c r="C2535" s="2"/>
-    </row>
-    <row r="2536" spans="1:3" ht="12.75">
-      <c r="A2536" s="1"/>
-      <c r="B2536" s="1"/>
-      <c r="C2536" s="2"/>
-    </row>
-    <row r="2537" spans="1:3" ht="12.75">
-      <c r="A2537" s="1"/>
-      <c r="B2537" s="1"/>
-      <c r="C2537" s="2"/>
-    </row>
-    <row r="2538" spans="1:3" ht="12.75">
-      <c r="A2538" s="1"/>
-      <c r="B2538" s="1"/>
-      <c r="C2538" s="2"/>
-    </row>
-    <row r="2539" spans="1:3" ht="12.75">
-      <c r="A2539" s="1"/>
-      <c r="B2539" s="1"/>
-      <c r="C2539" s="2"/>
-    </row>
-    <row r="2540" spans="1:3" ht="12.75">
-      <c r="A2540" s="1"/>
-      <c r="B2540" s="1"/>
-      <c r="C2540" s="2"/>
-    </row>
-    <row r="2541" spans="1:3" ht="12.75">
-      <c r="A2541" s="1"/>
-      <c r="B2541" s="1"/>
-      <c r="C2541" s="2"/>
-    </row>
-    <row r="2542" spans="1:3" ht="12.75">
-      <c r="A2542" s="1"/>
-      <c r="B2542" s="1"/>
-      <c r="C2542" s="2"/>
-    </row>
-    <row r="2543" spans="1:3" ht="12.75">
-      <c r="A2543" s="1"/>
-      <c r="B2543" s="1"/>
-      <c r="C2543" s="2"/>
-    </row>
-    <row r="2544" spans="1:3" ht="12.75">
-      <c r="A2544" s="1"/>
-      <c r="B2544" s="1"/>
-      <c r="C2544" s="2"/>
-    </row>
-    <row r="2545" spans="1:3" ht="12.75">
-      <c r="A2545" s="1"/>
-      <c r="B2545" s="1"/>
-      <c r="C2545" s="2"/>
-    </row>
-    <row r="2546" spans="1:3" ht="12.75">
-      <c r="A2546" s="1"/>
-      <c r="B2546" s="1"/>
-      <c r="C2546" s="2"/>
-    </row>
-    <row r="2547" spans="1:3" ht="12.75">
-      <c r="A2547" s="1"/>
-      <c r="B2547" s="1"/>
-      <c r="C2547" s="2"/>
-    </row>
-    <row r="2548" spans="1:3" ht="12.75">
-      <c r="A2548" s="1"/>
-      <c r="B2548" s="1"/>
-      <c r="C2548" s="2"/>
-    </row>
-    <row r="2549" spans="1:3" ht="12.75">
-      <c r="A2549" s="1"/>
-      <c r="B2549" s="1"/>
-      <c r="C2549" s="2"/>
-    </row>
-    <row r="2550" spans="1:3" ht="12.75">
-      <c r="A2550" s="1"/>
-      <c r="B2550" s="1"/>
-      <c r="C2550" s="2"/>
-    </row>
-    <row r="2551" spans="1:3" ht="12.75">
-      <c r="A2551" s="1"/>
-      <c r="B2551" s="1"/>
-      <c r="C2551" s="2"/>
-    </row>
-    <row r="2552" spans="1:3" ht="12.75">
-      <c r="A2552" s="1"/>
-      <c r="B2552" s="1"/>
-      <c r="C2552" s="2"/>
-    </row>
-    <row r="2553" spans="1:3" ht="12.75">
-      <c r="A2553" s="1"/>
-      <c r="B2553" s="1"/>
-      <c r="C2553" s="2"/>
-    </row>
-    <row r="2554" spans="1:3" ht="12.75">
-      <c r="A2554" s="1"/>
-      <c r="B2554" s="1"/>
-      <c r="C2554" s="2"/>
-    </row>
-    <row r="2555" spans="1:3" ht="12.75">
-      <c r="A2555" s="1"/>
-      <c r="B2555" s="1"/>
-      <c r="C2555" s="2"/>
-    </row>
-    <row r="2556" spans="1:3" ht="12.75">
-      <c r="A2556" s="1"/>
-      <c r="B2556" s="1"/>
-      <c r="C2556" s="2"/>
-    </row>
-    <row r="2557" spans="1:3" ht="12.75">
-      <c r="A2557" s="1"/>
-      <c r="B2557" s="1"/>
-      <c r="C2557" s="2"/>
-    </row>
-    <row r="2558" spans="1:3" ht="12.75">
-      <c r="A2558" s="1"/>
-      <c r="B2558" s="1"/>
-      <c r="C2558" s="2"/>
-    </row>
-    <row r="2559" spans="1:3" ht="12.75">
-      <c r="A2559" s="1"/>
-      <c r="B2559" s="1"/>
-      <c r="C2559" s="2"/>
-    </row>
-    <row r="2560" spans="1:3" ht="12.75">
-      <c r="A2560" s="1"/>
-      <c r="B2560" s="1"/>
-      <c r="C2560" s="2"/>
-    </row>
-    <row r="2561" spans="1:3" ht="12.75">
-      <c r="A2561" s="1"/>
-      <c r="B2561" s="1"/>
-      <c r="C2561" s="2"/>
-    </row>
-    <row r="2562" spans="1:3" ht="12.75">
-      <c r="A2562" s="1"/>
-      <c r="B2562" s="1"/>
-      <c r="C2562" s="2"/>
-    </row>
-    <row r="2563" spans="1:3" ht="12.75">
-      <c r="A2563" s="1"/>
-      <c r="B2563" s="1"/>
-      <c r="C2563" s="2"/>
-    </row>
-    <row r="2564" spans="1:3" ht="12.75">
-      <c r="A2564" s="1"/>
-      <c r="B2564" s="1"/>
-      <c r="C2564" s="2"/>
-    </row>
-    <row r="2565" spans="1:3" ht="12.75">
-      <c r="A2565" s="1"/>
-      <c r="B2565" s="1"/>
-      <c r="C2565" s="2"/>
-    </row>
-    <row r="2566" spans="1:3" ht="12.75">
-      <c r="A2566" s="1"/>
-      <c r="B2566" s="1"/>
-      <c r="C2566" s="2"/>
-    </row>
-    <row r="2567" spans="1:3" ht="12.75">
-      <c r="A2567" s="1"/>
-      <c r="B2567" s="1"/>
-      <c r="C2567" s="2"/>
-    </row>
-    <row r="2568" spans="1:3" ht="12.75">
-      <c r="A2568" s="1"/>
-      <c r="B2568" s="1"/>
-      <c r="C2568" s="2"/>
-    </row>
-    <row r="2569" spans="1:3" ht="12.75">
-      <c r="A2569" s="1"/>
-      <c r="B2569" s="1"/>
-      <c r="C2569" s="2"/>
-    </row>
-    <row r="2570" spans="1:3" ht="12.75">
-      <c r="A2570" s="1"/>
-      <c r="B2570" s="1"/>
-      <c r="C2570" s="2"/>
-    </row>
-    <row r="2571" spans="1:3" ht="12.75">
-      <c r="A2571" s="1"/>
-      <c r="B2571" s="1"/>
-      <c r="C2571" s="2"/>
-    </row>
-    <row r="2572" spans="1:3" ht="12.75">
-      <c r="A2572" s="1"/>
-      <c r="B2572" s="1"/>
-      <c r="C2572" s="2"/>
-    </row>
-    <row r="2573" spans="1:3" ht="12.75">
-      <c r="A2573" s="1"/>
-      <c r="B2573" s="1"/>
-      <c r="C2573" s="2"/>
-    </row>
-    <row r="2574" spans="1:3" ht="12.75">
-      <c r="A2574" s="1"/>
-      <c r="B2574" s="1"/>
-      <c r="C2574" s="2"/>
-    </row>
-    <row r="2575" spans="1:3" ht="12.75">
-      <c r="A2575" s="1"/>
-      <c r="B2575" s="1"/>
-      <c r="C2575" s="2"/>
-    </row>
-    <row r="2576" spans="1:3" ht="12.75">
-      <c r="A2576" s="1"/>
-      <c r="B2576" s="1"/>
-      <c r="C2576" s="2"/>
-    </row>
-    <row r="2577" spans="1:3" ht="12.75">
-      <c r="A2577" s="1"/>
-      <c r="B2577" s="1"/>
-      <c r="C2577" s="2"/>
-    </row>
-    <row r="2578" spans="1:3" ht="12.75">
-      <c r="A2578" s="1"/>
-      <c r="B2578" s="1"/>
-      <c r="C2578" s="2"/>
-    </row>
-    <row r="2579" spans="1:3" ht="12.75">
-      <c r="A2579" s="1"/>
-      <c r="B2579" s="1"/>
-      <c r="C2579" s="2"/>
-    </row>
-    <row r="2580" spans="1:3" ht="12.75">
-      <c r="A2580" s="1"/>
-      <c r="B2580" s="1"/>
-      <c r="C2580" s="2"/>
-    </row>
-    <row r="2581" spans="1:3" ht="12.75">
-      <c r="A2581" s="1"/>
-      <c r="B2581" s="1"/>
-      <c r="C2581" s="2"/>
-    </row>
-    <row r="2582" spans="1:3" ht="12.75">
-      <c r="A2582" s="1"/>
-      <c r="B2582" s="1"/>
-      <c r="C2582" s="2"/>
-    </row>
-    <row r="2583" spans="1:3" ht="12.75">
-      <c r="A2583" s="1"/>
-      <c r="B2583" s="1"/>
-      <c r="C2583" s="2"/>
-    </row>
-    <row r="2584" spans="1:3" ht="12.75">
-      <c r="A2584" s="1"/>
-      <c r="B2584" s="1"/>
-      <c r="C2584" s="2"/>
-    </row>
-    <row r="2585" spans="1:3" ht="12.75">
-      <c r="A2585" s="1"/>
-      <c r="B2585" s="1"/>
-      <c r="C2585" s="2"/>
-    </row>
-    <row r="2586" spans="1:3" ht="12.75">
-      <c r="A2586" s="1"/>
-      <c r="B2586" s="1"/>
-      <c r="C2586" s="2"/>
-    </row>
-    <row r="2587" spans="1:3" ht="12.75">
-      <c r="A2587" s="1"/>
-      <c r="B2587" s="1"/>
-      <c r="C2587" s="2"/>
-    </row>
-    <row r="2588" spans="1:3" ht="12.75">
-      <c r="A2588" s="1"/>
-      <c r="B2588" s="1"/>
-      <c r="C2588" s="2"/>
-    </row>
-    <row r="2589" spans="1:3" ht="12.75">
-      <c r="A2589" s="1"/>
-      <c r="B2589" s="1"/>
-      <c r="C2589" s="2"/>
-    </row>
-    <row r="2590" spans="1:3" ht="12.75">
-      <c r="A2590" s="1"/>
-      <c r="B2590" s="1"/>
-      <c r="C2590" s="2"/>
-    </row>
-    <row r="2591" spans="1:3" ht="12.75">
-      <c r="A2591" s="1"/>
-      <c r="B2591" s="1"/>
-      <c r="C2591" s="2"/>
-    </row>
-    <row r="2592" spans="1:3" ht="12.75">
-      <c r="A2592" s="1"/>
-      <c r="B2592" s="1"/>
-      <c r="C2592" s="2"/>
-    </row>
-    <row r="2593" spans="1:3" ht="12.75">
-      <c r="A2593" s="1"/>
-      <c r="B2593" s="1"/>
-      <c r="C2593" s="2"/>
-    </row>
-    <row r="2594" spans="1:3" ht="12.75">
-      <c r="A2594" s="1"/>
-      <c r="B2594" s="1"/>
-      <c r="C2594" s="2"/>
-    </row>
-    <row r="2595" spans="1:3" ht="12.75">
-      <c r="A2595" s="1"/>
-      <c r="B2595" s="1"/>
-      <c r="C2595" s="2"/>
-    </row>
-    <row r="2596" spans="1:3" ht="12.75">
-      <c r="A2596" s="1"/>
-      <c r="B2596" s="1"/>
-      <c r="C2596" s="2"/>
-    </row>
-    <row r="2597" spans="1:3" ht="12.75">
-      <c r="A2597" s="1"/>
-      <c r="B2597" s="1"/>
-      <c r="C2597" s="2"/>
-    </row>
-    <row r="2598" spans="1:3" ht="12.75">
-      <c r="A2598" s="1"/>
-      <c r="B2598" s="1"/>
-      <c r="C2598" s="2"/>
-    </row>
-    <row r="2599" spans="1:3" ht="12.75">
-      <c r="A2599" s="1"/>
-      <c r="B2599" s="1"/>
-      <c r="C2599" s="2"/>
-    </row>
-    <row r="2600" spans="1:3" ht="12.75">
-      <c r="A2600" s="1"/>
-      <c r="B2600" s="1"/>
-      <c r="C2600" s="2"/>
-    </row>
-    <row r="2601" spans="1:3" ht="12.75">
-      <c r="A2601" s="1"/>
-      <c r="B2601" s="1"/>
-      <c r="C2601" s="2"/>
-    </row>
-    <row r="2602" spans="1:3" ht="12.75">
-      <c r="A2602" s="1"/>
-      <c r="B2602" s="1"/>
-      <c r="C2602" s="2"/>
-    </row>
-    <row r="2603" spans="1:3" ht="12.75">
-      <c r="A2603" s="1"/>
-      <c r="B2603" s="1"/>
-      <c r="C2603" s="2"/>
-    </row>
-    <row r="2604" spans="1:3" ht="12.75">
-      <c r="A2604" s="1"/>
-      <c r="B2604" s="1"/>
-      <c r="C2604" s="2"/>
-    </row>
-    <row r="2605" spans="1:3" ht="12.75">
-      <c r="A2605" s="1"/>
-      <c r="B2605" s="1"/>
-      <c r="C2605" s="2"/>
-    </row>
-    <row r="2606" spans="1:3" ht="12.75">
-      <c r="A2606" s="1"/>
-      <c r="B2606" s="1"/>
-      <c r="C2606" s="2"/>
-    </row>
-    <row r="2607" spans="1:3" ht="12.75">
-      <c r="A2607" s="1"/>
-      <c r="B2607" s="1"/>
-      <c r="C2607" s="2"/>
-    </row>
-    <row r="2608" spans="1:3" ht="12.75">
-      <c r="A2608" s="1"/>
-      <c r="B2608" s="1"/>
-      <c r="C2608" s="2"/>
-    </row>
-    <row r="2609" spans="1:3" ht="12.75">
-      <c r="A2609" s="1"/>
-      <c r="B2609" s="1"/>
-      <c r="C2609" s="2"/>
-    </row>
-    <row r="2610" spans="1:3" ht="12.75">
-      <c r="A2610" s="1"/>
-      <c r="B2610" s="1"/>
-      <c r="C2610" s="2"/>
-    </row>
-    <row r="2611" spans="1:3" ht="12.75">
-      <c r="A2611" s="1"/>
-      <c r="B2611" s="1"/>
-      <c r="C2611" s="2"/>
-    </row>
-    <row r="2612" spans="1:3" ht="12.75">
-      <c r="A2612" s="1"/>
-      <c r="B2612" s="1"/>
-      <c r="C2612" s="2"/>
-    </row>
-    <row r="2613" spans="1:3" ht="12.75">
-      <c r="A2613" s="1"/>
-      <c r="B2613" s="1"/>
-      <c r="C2613" s="2"/>
-    </row>
-    <row r="2614" spans="1:3" ht="12.75">
-      <c r="A2614" s="1"/>
-      <c r="B2614" s="1"/>
-      <c r="C2614" s="2"/>
-    </row>
-    <row r="2615" spans="1:3" ht="12.75">
-      <c r="A2615" s="1"/>
-      <c r="B2615" s="1"/>
-      <c r="C2615" s="2"/>
-    </row>
-    <row r="2616" spans="1:3" ht="12.75">
-      <c r="A2616" s="1"/>
-      <c r="B2616" s="1"/>
-      <c r="C2616" s="2"/>
-    </row>
-    <row r="2617" spans="1:3" ht="12.75">
-      <c r="A2617" s="1"/>
-      <c r="B2617" s="1"/>
-      <c r="C2617" s="2"/>
-    </row>
-    <row r="2618" spans="1:3" ht="12.75">
-      <c r="A2618" s="1"/>
-      <c r="B2618" s="1"/>
-      <c r="C2618" s="2"/>
-    </row>
-    <row r="2619" spans="1:3" ht="12.75">
-      <c r="A2619" s="1"/>
-      <c r="B2619" s="1"/>
-      <c r="C2619" s="2"/>
-    </row>
-    <row r="2620" spans="1:3" ht="12.75">
-      <c r="A2620" s="1"/>
-      <c r="B2620" s="1"/>
-      <c r="C2620" s="2"/>
-    </row>
-    <row r="2621" spans="1:3" ht="12.75">
-      <c r="A2621" s="1"/>
-      <c r="B2621" s="1"/>
-      <c r="C2621" s="2"/>
-    </row>
-    <row r="2622" spans="1:3" ht="12.75">
-      <c r="A2622" s="1"/>
-      <c r="B2622" s="1"/>
-      <c r="C2622" s="2"/>
-    </row>
-    <row r="2623" spans="1:3" ht="12.75">
-      <c r="A2623" s="1"/>
-      <c r="B2623" s="1"/>
-      <c r="C2623" s="2"/>
-    </row>
-    <row r="2624" spans="1:3" ht="12.75">
-      <c r="A2624" s="1"/>
-      <c r="B2624" s="1"/>
-      <c r="C2624" s="2"/>
-    </row>
-    <row r="2625" spans="1:3" ht="12.75">
-      <c r="A2625" s="1"/>
-      <c r="B2625" s="1"/>
-      <c r="C2625" s="2"/>
-    </row>
-    <row r="2626" spans="1:3" ht="12.75">
-      <c r="A2626" s="1"/>
-      <c r="B2626" s="1"/>
-      <c r="C2626" s="2"/>
-    </row>
-    <row r="2627" spans="1:3" ht="12.75">
-      <c r="A2627" s="1"/>
-      <c r="B2627" s="1"/>
-      <c r="C2627" s="2"/>
-    </row>
-    <row r="2628" spans="1:3" ht="12.75">
-      <c r="A2628" s="1"/>
-      <c r="B2628" s="1"/>
-      <c r="C2628" s="2"/>
-    </row>
-    <row r="2629" spans="1:3" ht="12.75">
-      <c r="A2629" s="1"/>
-      <c r="B2629" s="1"/>
-      <c r="C2629" s="2"/>
-    </row>
-    <row r="2630" spans="1:3" ht="12.75">
-      <c r="A2630" s="1"/>
-      <c r="B2630" s="1"/>
-      <c r="C2630" s="2"/>
-    </row>
-    <row r="2631" spans="1:3" ht="12.75">
-      <c r="A2631" s="1"/>
-      <c r="B2631" s="1"/>
-      <c r="C2631" s="2"/>
-    </row>
-    <row r="2632" spans="1:3" ht="12.75">
-      <c r="A2632" s="1"/>
-      <c r="B2632" s="1"/>
-      <c r="C2632" s="2"/>
-    </row>
-    <row r="2633" spans="1:3" ht="12.75">
-      <c r="A2633" s="1"/>
-      <c r="B2633" s="1"/>
-      <c r="C2633" s="2"/>
-    </row>
-    <row r="2634" spans="1:3" ht="12.75">
-      <c r="A2634" s="1"/>
-      <c r="B2634" s="1"/>
-      <c r="C2634" s="2"/>
-    </row>
-    <row r="2635" spans="1:3" ht="12.75">
-      <c r="A2635" s="1"/>
-      <c r="B2635" s="1"/>
-      <c r="C2635" s="2"/>
-    </row>
-    <row r="2636" spans="1:3" ht="12.75">
-      <c r="A2636" s="1"/>
-      <c r="B2636" s="1"/>
-      <c r="C2636" s="2"/>
-    </row>
-    <row r="2637" spans="1:3" ht="12.75">
-      <c r="A2637" s="1"/>
-      <c r="B2637" s="1"/>
-      <c r="C2637" s="2"/>
-    </row>
-    <row r="2638" spans="1:3" ht="12.75">
-      <c r="A2638" s="1"/>
-      <c r="B2638" s="1"/>
-      <c r="C2638" s="2"/>
-    </row>
-    <row r="2639" spans="1:3" ht="12.75">
-      <c r="A2639" s="1"/>
-      <c r="B2639" s="1"/>
-      <c r="C2639" s="2"/>
-    </row>
-    <row r="2640" spans="1:3" ht="12.75">
-      <c r="A2640" s="1"/>
-      <c r="B2640" s="1"/>
-      <c r="C2640" s="2"/>
-    </row>
-    <row r="2641" spans="1:3" ht="12.75">
-      <c r="A2641" s="1"/>
-      <c r="B2641" s="1"/>
-      <c r="C2641" s="2"/>
-    </row>
-    <row r="2642" spans="1:3" ht="12.75">
-      <c r="A2642" s="1"/>
-      <c r="B2642" s="1"/>
-      <c r="C2642" s="2"/>
-    </row>
-    <row r="2643" spans="1:3" ht="12.75">
-      <c r="A2643" s="1"/>
-      <c r="B2643" s="1"/>
-      <c r="C2643" s="2"/>
-    </row>
-    <row r="2644" spans="1:3" ht="12.75">
-      <c r="A2644" s="1"/>
-      <c r="B2644" s="1"/>
-      <c r="C2644" s="2"/>
-    </row>
-    <row r="2645" spans="1:3" ht="12.75">
-      <c r="A2645" s="1"/>
-      <c r="B2645" s="1"/>
-      <c r="C2645" s="2"/>
-    </row>
-    <row r="2646" spans="1:3" ht="12.75">
-      <c r="A2646" s="1"/>
-      <c r="B2646" s="1"/>
-      <c r="C2646" s="2"/>
-    </row>
-    <row r="2647" spans="1:3" ht="12.75">
-      <c r="A2647" s="1"/>
-      <c r="B2647" s="1"/>
-      <c r="C2647" s="2"/>
-    </row>
-    <row r="2648" spans="1:3" ht="12.75">
-      <c r="A2648" s="1"/>
-      <c r="B2648" s="1"/>
-      <c r="C2648" s="2"/>
-    </row>
-    <row r="2649" spans="1:3" ht="12.75">
-      <c r="A2649" s="1"/>
-      <c r="B2649" s="1"/>
-      <c r="C2649" s="2"/>
-    </row>
-    <row r="2650" spans="1:3" ht="12.75">
-      <c r="A2650" s="1"/>
-      <c r="B2650" s="1"/>
-      <c r="C2650" s="2"/>
-    </row>
-    <row r="2651" spans="1:3" ht="12.75">
-      <c r="A2651" s="1"/>
-      <c r="B2651" s="1"/>
-      <c r="C2651" s="2"/>
-    </row>
-    <row r="2652" spans="1:3" ht="12.75">
-      <c r="A2652" s="1"/>
-      <c r="B2652" s="1"/>
-      <c r="C2652" s="2"/>
-    </row>
-    <row r="2653" spans="1:3" ht="12.75">
-      <c r="A2653" s="1"/>
-      <c r="B2653" s="1"/>
-      <c r="C2653" s="2"/>
-    </row>
-    <row r="2654" spans="1:3" ht="12.75">
-      <c r="A2654" s="1"/>
-      <c r="B2654" s="1"/>
-      <c r="C2654" s="2"/>
-    </row>
-    <row r="2655" spans="1:3" ht="12.75">
-      <c r="A2655" s="1"/>
-      <c r="B2655" s="1"/>
-      <c r="C2655" s="2"/>
-    </row>
-    <row r="2656" spans="1:3" ht="12.75">
-      <c r="A2656" s="1"/>
-      <c r="B2656" s="1"/>
-      <c r="C2656" s="2"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C2656">
+  <conditionalFormatting sqref="C1:C1890">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(C:C, C1)&gt;1</formula>
     </cfRule>

</xml_diff>